<commit_message>
updated outputs with additional assigned Trends
</commit_message>
<xml_diff>
--- a/ModelAggregation/output/TrendStatusText_Final2025-06-09.xlsx
+++ b/ModelAggregation/output/TrendStatusText_Final2025-06-09.xlsx
@@ -2091,7 +2091,9 @@
       <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="G3"/>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
       <c r="H3" t="b">
         <v>0</v>
       </c>
@@ -2205,7 +2207,9 @@
       <c r="F7" t="s">
         <v>24</v>
       </c>
-      <c r="G7"/>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
       <c r="H7" t="b">
         <v>0</v>
       </c>
@@ -2232,7 +2236,9 @@
       <c r="F8" t="s">
         <v>27</v>
       </c>
-      <c r="G8"/>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
       <c r="H8" t="b">
         <v>0</v>
       </c>
@@ -2288,7 +2294,9 @@
       <c r="F10" t="s">
         <v>32</v>
       </c>
-      <c r="G10"/>
+      <c r="G10" t="n">
+        <v>2</v>
+      </c>
       <c r="H10" t="b">
         <v>0</v>
       </c>
@@ -2315,7 +2323,9 @@
       <c r="F11" t="s">
         <v>34</v>
       </c>
-      <c r="G11"/>
+      <c r="G11" t="n">
+        <v>2</v>
+      </c>
       <c r="H11" t="b">
         <v>0</v>
       </c>
@@ -2342,7 +2352,9 @@
       <c r="F12" t="s">
         <v>36</v>
       </c>
-      <c r="G12"/>
+      <c r="G12" t="n">
+        <v>2</v>
+      </c>
       <c r="H12" t="b">
         <v>0</v>
       </c>
@@ -2369,7 +2381,9 @@
       <c r="F13" t="s">
         <v>39</v>
       </c>
-      <c r="G13"/>
+      <c r="G13" t="n">
+        <v>2</v>
+      </c>
       <c r="H13" t="b">
         <v>0</v>
       </c>
@@ -2396,7 +2410,9 @@
       <c r="F14" t="s">
         <v>41</v>
       </c>
-      <c r="G14"/>
+      <c r="G14" t="n">
+        <v>2</v>
+      </c>
       <c r="H14" t="b">
         <v>0</v>
       </c>
@@ -2423,7 +2439,9 @@
       <c r="F15" t="s">
         <v>43</v>
       </c>
-      <c r="G15"/>
+      <c r="G15" t="n">
+        <v>2</v>
+      </c>
       <c r="H15" t="b">
         <v>0</v>
       </c>
@@ -2508,7 +2526,9 @@
       <c r="F18" t="s">
         <v>47</v>
       </c>
-      <c r="G18"/>
+      <c r="G18" t="n">
+        <v>2</v>
+      </c>
       <c r="H18" t="b">
         <v>0</v>
       </c>
@@ -2622,7 +2642,9 @@
       <c r="F22" t="s">
         <v>51</v>
       </c>
-      <c r="G22"/>
+      <c r="G22" t="n">
+        <v>3</v>
+      </c>
       <c r="H22" t="b">
         <v>1</v>
       </c>
@@ -2649,7 +2671,9 @@
       <c r="F23" t="s">
         <v>52</v>
       </c>
-      <c r="G23"/>
+      <c r="G23" t="n">
+        <v>3</v>
+      </c>
       <c r="H23" t="b">
         <v>1</v>
       </c>
@@ -2705,7 +2729,9 @@
       <c r="F25" t="s">
         <v>54</v>
       </c>
-      <c r="G25"/>
+      <c r="G25" t="n">
+        <v>2</v>
+      </c>
       <c r="H25" t="b">
         <v>0</v>
       </c>
@@ -2732,7 +2758,9 @@
       <c r="F26" t="s">
         <v>55</v>
       </c>
-      <c r="G26"/>
+      <c r="G26" t="n">
+        <v>2</v>
+      </c>
       <c r="H26" t="b">
         <v>0</v>
       </c>
@@ -2759,7 +2787,9 @@
       <c r="F27" t="s">
         <v>36</v>
       </c>
-      <c r="G27"/>
+      <c r="G27" t="n">
+        <v>2</v>
+      </c>
       <c r="H27" t="b">
         <v>0</v>
       </c>
@@ -2844,7 +2874,9 @@
       <c r="F30" t="s">
         <v>43</v>
       </c>
-      <c r="G30"/>
+      <c r="G30" t="n">
+        <v>2</v>
+      </c>
       <c r="H30" t="b">
         <v>0</v>
       </c>
@@ -3045,7 +3077,9 @@
       <c r="F37" t="s">
         <v>62</v>
       </c>
-      <c r="G37"/>
+      <c r="G37" t="n">
+        <v>3</v>
+      </c>
       <c r="H37" t="b">
         <v>1</v>
       </c>
@@ -3072,7 +3106,9 @@
       <c r="F38" t="s">
         <v>52</v>
       </c>
-      <c r="G38"/>
+      <c r="G38" t="n">
+        <v>3</v>
+      </c>
       <c r="H38" t="b">
         <v>1</v>
       </c>
@@ -3128,7 +3164,9 @@
       <c r="F40" t="s">
         <v>64</v>
       </c>
-      <c r="G40"/>
+      <c r="G40" t="n">
+        <v>2</v>
+      </c>
       <c r="H40" t="b">
         <v>0</v>
       </c>
@@ -3155,7 +3193,9 @@
       <c r="F41" t="s">
         <v>65</v>
       </c>
-      <c r="G41"/>
+      <c r="G41" t="n">
+        <v>2</v>
+      </c>
       <c r="H41" t="b">
         <v>0</v>
       </c>
@@ -3182,7 +3222,9 @@
       <c r="F42" t="s">
         <v>36</v>
       </c>
-      <c r="G42"/>
+      <c r="G42" t="n">
+        <v>2</v>
+      </c>
       <c r="H42" t="b">
         <v>0</v>
       </c>
@@ -3267,7 +3309,9 @@
       <c r="F45" t="s">
         <v>43</v>
       </c>
-      <c r="G45"/>
+      <c r="G45" t="n">
+        <v>2</v>
+      </c>
       <c r="H45" t="b">
         <v>0</v>
       </c>
@@ -3468,7 +3512,9 @@
       <c r="F52" t="s">
         <v>75</v>
       </c>
-      <c r="G52"/>
+      <c r="G52" t="n">
+        <v>2</v>
+      </c>
       <c r="H52" t="b">
         <v>0</v>
       </c>
@@ -3495,7 +3541,9 @@
       <c r="F53" t="s">
         <v>76</v>
       </c>
-      <c r="G53"/>
+      <c r="G53" t="n">
+        <v>2</v>
+      </c>
       <c r="H53" t="b">
         <v>0</v>
       </c>
@@ -3551,7 +3599,9 @@
       <c r="F55" t="s">
         <v>78</v>
       </c>
-      <c r="G55"/>
+      <c r="G55" t="n">
+        <v>2</v>
+      </c>
       <c r="H55" t="b">
         <v>0</v>
       </c>
@@ -3578,7 +3628,9 @@
       <c r="F56" t="s">
         <v>79</v>
       </c>
-      <c r="G56"/>
+      <c r="G56" t="n">
+        <v>2</v>
+      </c>
       <c r="H56" t="b">
         <v>0</v>
       </c>
@@ -3605,7 +3657,9 @@
       <c r="F57" t="s">
         <v>36</v>
       </c>
-      <c r="G57"/>
+      <c r="G57" t="n">
+        <v>2</v>
+      </c>
       <c r="H57" t="b">
         <v>0</v>
       </c>
@@ -3632,7 +3686,9 @@
       <c r="F58" t="s">
         <v>39</v>
       </c>
-      <c r="G58"/>
+      <c r="G58" t="n">
+        <v>2</v>
+      </c>
       <c r="H58" t="b">
         <v>0</v>
       </c>
@@ -3659,7 +3715,9 @@
       <c r="F59" t="s">
         <v>41</v>
       </c>
-      <c r="G59"/>
+      <c r="G59" t="n">
+        <v>2</v>
+      </c>
       <c r="H59" t="b">
         <v>0</v>
       </c>
@@ -3686,7 +3744,9 @@
       <c r="F60" t="s">
         <v>43</v>
       </c>
-      <c r="G60"/>
+      <c r="G60" t="n">
+        <v>2</v>
+      </c>
       <c r="H60" t="b">
         <v>0</v>
       </c>
@@ -3713,7 +3773,9 @@
       <c r="F61" t="s">
         <v>80</v>
       </c>
-      <c r="G61"/>
+      <c r="G61" t="n">
+        <v>2</v>
+      </c>
       <c r="H61" t="b">
         <v>0</v>
       </c>
@@ -3885,7 +3947,9 @@
       <c r="F67" t="s">
         <v>86</v>
       </c>
-      <c r="G67"/>
+      <c r="G67" t="n">
+        <v>2</v>
+      </c>
       <c r="H67" t="b">
         <v>0</v>
       </c>
@@ -3912,7 +3976,9 @@
       <c r="F68" t="s">
         <v>87</v>
       </c>
-      <c r="G68"/>
+      <c r="G68" t="n">
+        <v>3</v>
+      </c>
       <c r="H68" t="b">
         <v>1</v>
       </c>
@@ -3968,7 +4034,9 @@
       <c r="F70" t="s">
         <v>89</v>
       </c>
-      <c r="G70"/>
+      <c r="G70" t="n">
+        <v>2</v>
+      </c>
       <c r="H70" t="b">
         <v>0</v>
       </c>
@@ -3995,7 +4063,9 @@
       <c r="F71" t="s">
         <v>90</v>
       </c>
-      <c r="G71"/>
+      <c r="G71" t="n">
+        <v>2</v>
+      </c>
       <c r="H71" t="b">
         <v>0</v>
       </c>
@@ -4022,7 +4092,9 @@
       <c r="F72" t="s">
         <v>36</v>
       </c>
-      <c r="G72"/>
+      <c r="G72" t="n">
+        <v>2</v>
+      </c>
       <c r="H72" t="b">
         <v>0</v>
       </c>
@@ -4049,7 +4121,9 @@
       <c r="F73" t="s">
         <v>39</v>
       </c>
-      <c r="G73"/>
+      <c r="G73" t="n">
+        <v>2</v>
+      </c>
       <c r="H73" t="b">
         <v>0</v>
       </c>
@@ -4076,7 +4150,9 @@
       <c r="F74" t="s">
         <v>41</v>
       </c>
-      <c r="G74"/>
+      <c r="G74" t="n">
+        <v>2</v>
+      </c>
       <c r="H74" t="b">
         <v>0</v>
       </c>
@@ -4103,7 +4179,9 @@
       <c r="F75" t="s">
         <v>91</v>
       </c>
-      <c r="G75"/>
+      <c r="G75" t="n">
+        <v>2</v>
+      </c>
       <c r="H75" t="b">
         <v>0</v>
       </c>
@@ -4159,7 +4237,9 @@
       <c r="F77" t="s">
         <v>95</v>
       </c>
-      <c r="G77"/>
+      <c r="G77" t="n">
+        <v>2</v>
+      </c>
       <c r="H77" t="b">
         <v>0</v>
       </c>
@@ -4215,7 +4295,9 @@
       <c r="F79" t="s">
         <v>97</v>
       </c>
-      <c r="G79"/>
+      <c r="G79" t="n">
+        <v>2</v>
+      </c>
       <c r="H79" t="b">
         <v>0</v>
       </c>
@@ -4242,7 +4324,9 @@
       <c r="F80" t="s">
         <v>98</v>
       </c>
-      <c r="G80"/>
+      <c r="G80" t="n">
+        <v>2</v>
+      </c>
       <c r="H80" t="b">
         <v>0</v>
       </c>
@@ -4269,7 +4353,9 @@
       <c r="F81" t="s">
         <v>99</v>
       </c>
-      <c r="G81"/>
+      <c r="G81" t="n">
+        <v>2</v>
+      </c>
       <c r="H81" t="b">
         <v>0</v>
       </c>
@@ -4296,7 +4382,9 @@
       <c r="F82" t="s">
         <v>100</v>
       </c>
-      <c r="G82"/>
+      <c r="G82" t="n">
+        <v>2</v>
+      </c>
       <c r="H82" t="b">
         <v>0</v>
       </c>
@@ -4323,7 +4411,9 @@
       <c r="F83" t="s">
         <v>101</v>
       </c>
-      <c r="G83"/>
+      <c r="G83" t="n">
+        <v>2</v>
+      </c>
       <c r="H83" t="b">
         <v>0</v>
       </c>
@@ -4379,7 +4469,9 @@
       <c r="F85" t="s">
         <v>103</v>
       </c>
-      <c r="G85"/>
+      <c r="G85" t="n">
+        <v>3</v>
+      </c>
       <c r="H85" t="b">
         <v>1</v>
       </c>
@@ -4435,7 +4527,9 @@
       <c r="F87" t="s">
         <v>36</v>
       </c>
-      <c r="G87"/>
+      <c r="G87" t="n">
+        <v>2</v>
+      </c>
       <c r="H87" t="b">
         <v>0</v>
       </c>
@@ -4462,7 +4556,9 @@
       <c r="F88" t="s">
         <v>39</v>
       </c>
-      <c r="G88"/>
+      <c r="G88" t="n">
+        <v>2</v>
+      </c>
       <c r="H88" t="b">
         <v>0</v>
       </c>
@@ -4489,7 +4585,9 @@
       <c r="F89" t="s">
         <v>41</v>
       </c>
-      <c r="G89"/>
+      <c r="G89" t="n">
+        <v>2</v>
+      </c>
       <c r="H89" t="b">
         <v>0</v>
       </c>
@@ -4516,7 +4614,9 @@
       <c r="F90" t="s">
         <v>43</v>
       </c>
-      <c r="G90"/>
+      <c r="G90" t="n">
+        <v>2</v>
+      </c>
       <c r="H90" t="b">
         <v>0</v>
       </c>
@@ -4543,7 +4643,9 @@
       <c r="F91" t="s">
         <v>105</v>
       </c>
-      <c r="G91"/>
+      <c r="G91" t="n">
+        <v>2</v>
+      </c>
       <c r="H91" t="b">
         <v>0</v>
       </c>
@@ -4715,7 +4817,9 @@
       <c r="F97" t="s">
         <v>111</v>
       </c>
-      <c r="G97"/>
+      <c r="G97" t="n">
+        <v>2</v>
+      </c>
       <c r="H97" t="b">
         <v>0</v>
       </c>
@@ -4742,7 +4846,9 @@
       <c r="F98" t="s">
         <v>112</v>
       </c>
-      <c r="G98"/>
+      <c r="G98" t="n">
+        <v>2</v>
+      </c>
       <c r="H98" t="b">
         <v>0</v>
       </c>
@@ -4798,7 +4904,9 @@
       <c r="F100" t="s">
         <v>114</v>
       </c>
-      <c r="G100"/>
+      <c r="G100" t="n">
+        <v>3</v>
+      </c>
       <c r="H100" t="b">
         <v>1</v>
       </c>
@@ -4825,7 +4933,9 @@
       <c r="F101" t="s">
         <v>115</v>
       </c>
-      <c r="G101"/>
+      <c r="G101" t="n">
+        <v>2</v>
+      </c>
       <c r="H101" t="b">
         <v>0</v>
       </c>
@@ -4852,7 +4962,9 @@
       <c r="F102" t="s">
         <v>36</v>
       </c>
-      <c r="G102"/>
+      <c r="G102" t="n">
+        <v>2</v>
+      </c>
       <c r="H102" t="b">
         <v>0</v>
       </c>
@@ -4879,7 +4991,9 @@
       <c r="F103" t="s">
         <v>39</v>
       </c>
-      <c r="G103"/>
+      <c r="G103" t="n">
+        <v>2</v>
+      </c>
       <c r="H103" t="b">
         <v>0</v>
       </c>
@@ -4906,7 +5020,9 @@
       <c r="F104" t="s">
         <v>41</v>
       </c>
-      <c r="G104"/>
+      <c r="G104" t="n">
+        <v>2</v>
+      </c>
       <c r="H104" t="b">
         <v>0</v>
       </c>
@@ -4933,7 +5049,9 @@
       <c r="F105" t="s">
         <v>43</v>
       </c>
-      <c r="G105"/>
+      <c r="G105" t="n">
+        <v>2</v>
+      </c>
       <c r="H105" t="b">
         <v>0</v>
       </c>
@@ -4960,7 +5078,9 @@
       <c r="F106" t="s">
         <v>116</v>
       </c>
-      <c r="G106"/>
+      <c r="G106" t="n">
+        <v>2</v>
+      </c>
       <c r="H106" t="b">
         <v>0</v>
       </c>
@@ -5132,7 +5252,9 @@
       <c r="F112" t="s">
         <v>123</v>
       </c>
-      <c r="G112"/>
+      <c r="G112" t="n">
+        <v>3</v>
+      </c>
       <c r="H112" t="b">
         <v>1</v>
       </c>
@@ -5159,7 +5281,9 @@
       <c r="F113" t="s">
         <v>124</v>
       </c>
-      <c r="G113"/>
+      <c r="G113" t="n">
+        <v>2</v>
+      </c>
       <c r="H113" t="b">
         <v>0</v>
       </c>
@@ -5215,7 +5339,9 @@
       <c r="F115" t="s">
         <v>126</v>
       </c>
-      <c r="G115"/>
+      <c r="G115" t="n">
+        <v>2</v>
+      </c>
       <c r="H115" t="b">
         <v>0</v>
       </c>
@@ -5242,7 +5368,9 @@
       <c r="F116" t="s">
         <v>127</v>
       </c>
-      <c r="G116"/>
+      <c r="G116" t="n">
+        <v>2</v>
+      </c>
       <c r="H116" t="b">
         <v>0</v>
       </c>
@@ -5269,7 +5397,9 @@
       <c r="F117" t="s">
         <v>36</v>
       </c>
-      <c r="G117"/>
+      <c r="G117" t="n">
+        <v>2</v>
+      </c>
       <c r="H117" t="b">
         <v>0</v>
       </c>
@@ -5296,7 +5426,9 @@
       <c r="F118" t="s">
         <v>128</v>
       </c>
-      <c r="G118"/>
+      <c r="G118" t="n">
+        <v>2</v>
+      </c>
       <c r="H118" t="b">
         <v>0</v>
       </c>
@@ -5323,7 +5455,9 @@
       <c r="F119" t="s">
         <v>129</v>
       </c>
-      <c r="G119"/>
+      <c r="G119" t="n">
+        <v>2</v>
+      </c>
       <c r="H119" t="b">
         <v>0</v>
       </c>
@@ -5350,7 +5484,9 @@
       <c r="F120" t="s">
         <v>130</v>
       </c>
-      <c r="G120"/>
+      <c r="G120" t="n">
+        <v>2</v>
+      </c>
       <c r="H120" t="b">
         <v>0</v>
       </c>
@@ -5551,7 +5687,9 @@
       <c r="F127" t="s">
         <v>137</v>
       </c>
-      <c r="G127"/>
+      <c r="G127" t="n">
+        <v>2</v>
+      </c>
       <c r="H127" t="b">
         <v>0</v>
       </c>
@@ -5578,7 +5716,9 @@
       <c r="F128" t="s">
         <v>138</v>
       </c>
-      <c r="G128"/>
+      <c r="G128" t="n">
+        <v>2</v>
+      </c>
       <c r="H128" t="b">
         <v>0</v>
       </c>
@@ -5634,7 +5774,9 @@
       <c r="F130" t="s">
         <v>140</v>
       </c>
-      <c r="G130"/>
+      <c r="G130" t="n">
+        <v>2</v>
+      </c>
       <c r="H130" t="b">
         <v>0</v>
       </c>
@@ -5661,7 +5803,9 @@
       <c r="F131" t="s">
         <v>141</v>
       </c>
-      <c r="G131"/>
+      <c r="G131" t="n">
+        <v>2</v>
+      </c>
       <c r="H131" t="b">
         <v>0</v>
       </c>
@@ -5688,7 +5832,9 @@
       <c r="F132" t="s">
         <v>36</v>
       </c>
-      <c r="G132"/>
+      <c r="G132" t="n">
+        <v>2</v>
+      </c>
       <c r="H132" t="b">
         <v>0</v>
       </c>
@@ -5715,7 +5861,9 @@
       <c r="F133" t="s">
         <v>39</v>
       </c>
-      <c r="G133"/>
+      <c r="G133" t="n">
+        <v>2</v>
+      </c>
       <c r="H133" t="b">
         <v>0</v>
       </c>
@@ -5742,7 +5890,9 @@
       <c r="F134" t="s">
         <v>41</v>
       </c>
-      <c r="G134"/>
+      <c r="G134" t="n">
+        <v>2</v>
+      </c>
       <c r="H134" t="b">
         <v>0</v>
       </c>
@@ -5769,7 +5919,9 @@
       <c r="F135" t="s">
         <v>43</v>
       </c>
-      <c r="G135"/>
+      <c r="G135" t="n">
+        <v>2</v>
+      </c>
       <c r="H135" t="b">
         <v>0</v>
       </c>
@@ -5825,7 +5977,9 @@
       <c r="F137" t="s">
         <v>144</v>
       </c>
-      <c r="G137"/>
+      <c r="G137" t="n">
+        <v>2</v>
+      </c>
       <c r="H137" t="b">
         <v>0</v>
       </c>
@@ -5968,7 +6122,9 @@
       <c r="F142" t="s">
         <v>148</v>
       </c>
-      <c r="G142"/>
+      <c r="G142" t="n">
+        <v>3</v>
+      </c>
       <c r="H142" t="b">
         <v>1</v>
       </c>
@@ -5995,7 +6151,9 @@
       <c r="F143" t="s">
         <v>149</v>
       </c>
-      <c r="G143"/>
+      <c r="G143" t="n">
+        <v>2</v>
+      </c>
       <c r="H143" t="b">
         <v>0</v>
       </c>
@@ -6051,7 +6209,9 @@
       <c r="F145" t="s">
         <v>151</v>
       </c>
-      <c r="G145"/>
+      <c r="G145" t="n">
+        <v>2</v>
+      </c>
       <c r="H145" t="b">
         <v>0</v>
       </c>
@@ -6078,7 +6238,9 @@
       <c r="F146" t="s">
         <v>152</v>
       </c>
-      <c r="G146"/>
+      <c r="G146" t="n">
+        <v>2</v>
+      </c>
       <c r="H146" t="b">
         <v>0</v>
       </c>
@@ -6105,7 +6267,9 @@
       <c r="F147" t="s">
         <v>36</v>
       </c>
-      <c r="G147"/>
+      <c r="G147" t="n">
+        <v>2</v>
+      </c>
       <c r="H147" t="b">
         <v>0</v>
       </c>
@@ -6132,7 +6296,9 @@
       <c r="F148" t="s">
         <v>39</v>
       </c>
-      <c r="G148"/>
+      <c r="G148" t="n">
+        <v>2</v>
+      </c>
       <c r="H148" t="b">
         <v>0</v>
       </c>
@@ -6159,7 +6325,9 @@
       <c r="F149" t="s">
         <v>41</v>
       </c>
-      <c r="G149"/>
+      <c r="G149" t="n">
+        <v>2</v>
+      </c>
       <c r="H149" t="b">
         <v>0</v>
       </c>
@@ -6186,7 +6354,9 @@
       <c r="F150" t="s">
         <v>43</v>
       </c>
-      <c r="G150"/>
+      <c r="G150" t="n">
+        <v>2</v>
+      </c>
       <c r="H150" t="b">
         <v>0</v>
       </c>
@@ -6213,7 +6383,9 @@
       <c r="F151" t="s">
         <v>153</v>
       </c>
-      <c r="G151"/>
+      <c r="G151" t="n">
+        <v>2</v>
+      </c>
       <c r="H151" t="b">
         <v>0</v>
       </c>
@@ -6385,7 +6557,9 @@
       <c r="F157" t="s">
         <v>158</v>
       </c>
-      <c r="G157"/>
+      <c r="G157" t="n">
+        <v>3</v>
+      </c>
       <c r="H157" t="b">
         <v>1</v>
       </c>
@@ -6412,7 +6586,9 @@
       <c r="F158" t="s">
         <v>159</v>
       </c>
-      <c r="G158"/>
+      <c r="G158" t="n">
+        <v>3</v>
+      </c>
       <c r="H158" t="b">
         <v>1</v>
       </c>
@@ -6468,7 +6644,9 @@
       <c r="F160" t="s">
         <v>161</v>
       </c>
-      <c r="G160"/>
+      <c r="G160" t="n">
+        <v>2</v>
+      </c>
       <c r="H160" t="b">
         <v>0</v>
       </c>
@@ -6495,7 +6673,9 @@
       <c r="F161" t="s">
         <v>162</v>
       </c>
-      <c r="G161"/>
+      <c r="G161" t="n">
+        <v>2</v>
+      </c>
       <c r="H161" t="b">
         <v>0</v>
       </c>
@@ -6522,7 +6702,9 @@
       <c r="F162" t="s">
         <v>36</v>
       </c>
-      <c r="G162"/>
+      <c r="G162" t="n">
+        <v>2</v>
+      </c>
       <c r="H162" t="b">
         <v>0</v>
       </c>
@@ -6549,7 +6731,9 @@
       <c r="F163" t="s">
         <v>39</v>
       </c>
-      <c r="G163"/>
+      <c r="G163" t="n">
+        <v>2</v>
+      </c>
       <c r="H163" t="b">
         <v>0</v>
       </c>
@@ -6576,7 +6760,9 @@
       <c r="F164" t="s">
         <v>41</v>
       </c>
-      <c r="G164"/>
+      <c r="G164" t="n">
+        <v>2</v>
+      </c>
       <c r="H164" t="b">
         <v>0</v>
       </c>
@@ -6603,7 +6789,9 @@
       <c r="F165" t="s">
         <v>43</v>
       </c>
-      <c r="G165"/>
+      <c r="G165" t="n">
+        <v>2</v>
+      </c>
       <c r="H165" t="b">
         <v>0</v>
       </c>
@@ -6659,7 +6847,9 @@
       <c r="F167" t="s">
         <v>165</v>
       </c>
-      <c r="G167"/>
+      <c r="G167" t="n">
+        <v>2</v>
+      </c>
       <c r="H167" t="b">
         <v>0</v>
       </c>
@@ -6686,7 +6876,9 @@
       <c r="F168" t="s">
         <v>166</v>
       </c>
-      <c r="G168"/>
+      <c r="G168" t="n">
+        <v>2</v>
+      </c>
       <c r="H168" t="b">
         <v>0</v>
       </c>
@@ -6800,7 +6992,9 @@
       <c r="F172" t="s">
         <v>169</v>
       </c>
-      <c r="G172"/>
+      <c r="G172" t="n">
+        <v>2</v>
+      </c>
       <c r="H172" t="b">
         <v>0</v>
       </c>
@@ -6827,7 +7021,9 @@
       <c r="F173" t="s">
         <v>170</v>
       </c>
-      <c r="G173"/>
+      <c r="G173" t="n">
+        <v>2</v>
+      </c>
       <c r="H173" t="b">
         <v>0</v>
       </c>
@@ -6883,7 +7079,9 @@
       <c r="F175" t="s">
         <v>172</v>
       </c>
-      <c r="G175"/>
+      <c r="G175" t="n">
+        <v>3</v>
+      </c>
       <c r="H175" t="b">
         <v>1</v>
       </c>
@@ -6910,7 +7108,9 @@
       <c r="F176" t="s">
         <v>173</v>
       </c>
-      <c r="G176"/>
+      <c r="G176" t="n">
+        <v>2</v>
+      </c>
       <c r="H176" t="b">
         <v>0</v>
       </c>
@@ -6937,7 +7137,9 @@
       <c r="F177" t="s">
         <v>36</v>
       </c>
-      <c r="G177"/>
+      <c r="G177" t="n">
+        <v>2</v>
+      </c>
       <c r="H177" t="b">
         <v>0</v>
       </c>
@@ -6964,7 +7166,9 @@
       <c r="F178" t="s">
         <v>39</v>
       </c>
-      <c r="G178"/>
+      <c r="G178" t="n">
+        <v>2</v>
+      </c>
       <c r="H178" t="b">
         <v>0</v>
       </c>
@@ -6991,7 +7195,9 @@
       <c r="F179" t="s">
         <v>41</v>
       </c>
-      <c r="G179"/>
+      <c r="G179" t="n">
+        <v>2</v>
+      </c>
       <c r="H179" t="b">
         <v>0</v>
       </c>
@@ -7018,7 +7224,9 @@
       <c r="F180" t="s">
         <v>43</v>
       </c>
-      <c r="G180"/>
+      <c r="G180" t="n">
+        <v>2</v>
+      </c>
       <c r="H180" t="b">
         <v>0</v>
       </c>
@@ -7045,7 +7253,9 @@
       <c r="F181" t="s">
         <v>174</v>
       </c>
-      <c r="G181"/>
+      <c r="G181" t="n">
+        <v>2</v>
+      </c>
       <c r="H181" t="b">
         <v>0</v>
       </c>
@@ -7217,7 +7427,9 @@
       <c r="F187" t="s">
         <v>180</v>
       </c>
-      <c r="G187"/>
+      <c r="G187" t="n">
+        <v>2</v>
+      </c>
       <c r="H187" t="b">
         <v>0</v>
       </c>
@@ -7244,7 +7456,9 @@
       <c r="F188" t="s">
         <v>181</v>
       </c>
-      <c r="G188"/>
+      <c r="G188" t="n">
+        <v>2</v>
+      </c>
       <c r="H188" t="b">
         <v>0</v>
       </c>
@@ -7300,7 +7514,9 @@
       <c r="F190" t="s">
         <v>183</v>
       </c>
-      <c r="G190"/>
+      <c r="G190" t="n">
+        <v>2</v>
+      </c>
       <c r="H190" t="b">
         <v>0</v>
       </c>
@@ -7327,7 +7543,9 @@
       <c r="F191" t="s">
         <v>184</v>
       </c>
-      <c r="G191"/>
+      <c r="G191" t="n">
+        <v>2</v>
+      </c>
       <c r="H191" t="b">
         <v>0</v>
       </c>
@@ -7354,7 +7572,9 @@
       <c r="F192" t="s">
         <v>36</v>
       </c>
-      <c r="G192"/>
+      <c r="G192" t="n">
+        <v>2</v>
+      </c>
       <c r="H192" t="b">
         <v>0</v>
       </c>
@@ -7497,7 +7717,9 @@
       <c r="F197" t="s">
         <v>190</v>
       </c>
-      <c r="G197"/>
+      <c r="G197" t="n">
+        <v>2</v>
+      </c>
       <c r="H197" t="b">
         <v>0</v>
       </c>
@@ -7640,7 +7862,9 @@
       <c r="F202" t="s">
         <v>193</v>
       </c>
-      <c r="G202"/>
+      <c r="G202" t="n">
+        <v>2</v>
+      </c>
       <c r="H202" t="b">
         <v>0</v>
       </c>
@@ -7667,7 +7891,9 @@
       <c r="F203" t="s">
         <v>194</v>
       </c>
-      <c r="G203"/>
+      <c r="G203" t="n">
+        <v>2</v>
+      </c>
       <c r="H203" t="b">
         <v>0</v>
       </c>
@@ -7723,7 +7949,9 @@
       <c r="F205" t="s">
         <v>196</v>
       </c>
-      <c r="G205"/>
+      <c r="G205" t="n">
+        <v>3</v>
+      </c>
       <c r="H205" t="b">
         <v>1</v>
       </c>
@@ -7779,7 +8007,9 @@
       <c r="F207" t="s">
         <v>36</v>
       </c>
-      <c r="G207"/>
+      <c r="G207" t="n">
+        <v>2</v>
+      </c>
       <c r="H207" t="b">
         <v>0</v>
       </c>
@@ -7806,7 +8036,9 @@
       <c r="F208" t="s">
         <v>39</v>
       </c>
-      <c r="G208"/>
+      <c r="G208" t="n">
+        <v>2</v>
+      </c>
       <c r="H208" t="b">
         <v>0</v>
       </c>
@@ -7833,7 +8065,9 @@
       <c r="F209" t="s">
         <v>41</v>
       </c>
-      <c r="G209"/>
+      <c r="G209" t="n">
+        <v>2</v>
+      </c>
       <c r="H209" t="b">
         <v>0</v>
       </c>
@@ -7860,7 +8094,9 @@
       <c r="F210" t="s">
         <v>43</v>
       </c>
-      <c r="G210"/>
+      <c r="G210" t="n">
+        <v>2</v>
+      </c>
       <c r="H210" t="b">
         <v>0</v>
       </c>
@@ -7887,7 +8123,9 @@
       <c r="F211" t="s">
         <v>198</v>
       </c>
-      <c r="G211"/>
+      <c r="G211" t="n">
+        <v>2</v>
+      </c>
       <c r="H211" t="b">
         <v>0</v>
       </c>
@@ -7914,7 +8152,9 @@
       <c r="F212" t="s">
         <v>200</v>
       </c>
-      <c r="G212"/>
+      <c r="G212" t="n">
+        <v>2</v>
+      </c>
       <c r="H212" t="b">
         <v>0</v>
       </c>
@@ -7941,7 +8181,9 @@
       <c r="F213" t="s">
         <v>201</v>
       </c>
-      <c r="G213"/>
+      <c r="G213" t="n">
+        <v>2</v>
+      </c>
       <c r="H213" t="b">
         <v>0</v>
       </c>
@@ -8055,7 +8297,9 @@
       <c r="F217" t="s">
         <v>205</v>
       </c>
-      <c r="G217"/>
+      <c r="G217" t="n">
+        <v>2</v>
+      </c>
       <c r="H217" t="b">
         <v>0</v>
       </c>
@@ -8082,7 +8326,9 @@
       <c r="F218" t="s">
         <v>206</v>
       </c>
-      <c r="G218"/>
+      <c r="G218" t="n">
+        <v>2</v>
+      </c>
       <c r="H218" t="b">
         <v>0</v>
       </c>
@@ -8138,7 +8384,9 @@
       <c r="F220" t="s">
         <v>208</v>
       </c>
-      <c r="G220"/>
+      <c r="G220" t="n">
+        <v>2</v>
+      </c>
       <c r="H220" t="b">
         <v>0</v>
       </c>
@@ -8165,7 +8413,9 @@
       <c r="F221" t="s">
         <v>209</v>
       </c>
-      <c r="G221"/>
+      <c r="G221" t="n">
+        <v>2</v>
+      </c>
       <c r="H221" t="b">
         <v>0</v>
       </c>
@@ -8192,7 +8442,9 @@
       <c r="F222" t="s">
         <v>36</v>
       </c>
-      <c r="G222"/>
+      <c r="G222" t="n">
+        <v>2</v>
+      </c>
       <c r="H222" t="b">
         <v>0</v>
       </c>
@@ -8219,7 +8471,9 @@
       <c r="F223" t="s">
         <v>39</v>
       </c>
-      <c r="G223"/>
+      <c r="G223" t="n">
+        <v>2</v>
+      </c>
       <c r="H223" t="b">
         <v>0</v>
       </c>
@@ -8246,7 +8500,9 @@
       <c r="F224" t="s">
         <v>41</v>
       </c>
-      <c r="G224"/>
+      <c r="G224" t="n">
+        <v>2</v>
+      </c>
       <c r="H224" t="b">
         <v>0</v>
       </c>
@@ -8273,7 +8529,9 @@
       <c r="F225" t="s">
         <v>43</v>
       </c>
-      <c r="G225"/>
+      <c r="G225" t="n">
+        <v>2</v>
+      </c>
       <c r="H225" t="b">
         <v>0</v>
       </c>
@@ -8300,7 +8558,9 @@
       <c r="F226" t="s">
         <v>210</v>
       </c>
-      <c r="G226"/>
+      <c r="G226" t="n">
+        <v>2</v>
+      </c>
       <c r="H226" t="b">
         <v>0</v>
       </c>
@@ -8472,7 +8732,9 @@
       <c r="F232" t="s">
         <v>216</v>
       </c>
-      <c r="G232"/>
+      <c r="G232" t="n">
+        <v>2</v>
+      </c>
       <c r="H232" t="b">
         <v>0</v>
       </c>
@@ -8499,7 +8761,9 @@
       <c r="F233" t="s">
         <v>217</v>
       </c>
-      <c r="G233"/>
+      <c r="G233" t="n">
+        <v>2</v>
+      </c>
       <c r="H233" t="b">
         <v>0</v>
       </c>
@@ -8555,7 +8819,9 @@
       <c r="F235" t="s">
         <v>219</v>
       </c>
-      <c r="G235"/>
+      <c r="G235" t="n">
+        <v>2</v>
+      </c>
       <c r="H235" t="b">
         <v>0</v>
       </c>
@@ -8582,7 +8848,9 @@
       <c r="F236" t="s">
         <v>220</v>
       </c>
-      <c r="G236"/>
+      <c r="G236" t="n">
+        <v>2</v>
+      </c>
       <c r="H236" t="b">
         <v>0</v>
       </c>
@@ -8609,7 +8877,9 @@
       <c r="F237" t="s">
         <v>36</v>
       </c>
-      <c r="G237"/>
+      <c r="G237" t="n">
+        <v>2</v>
+      </c>
       <c r="H237" t="b">
         <v>0</v>
       </c>
@@ -8636,7 +8906,9 @@
       <c r="F238" t="s">
         <v>39</v>
       </c>
-      <c r="G238"/>
+      <c r="G238" t="n">
+        <v>2</v>
+      </c>
       <c r="H238" t="b">
         <v>0</v>
       </c>
@@ -8663,7 +8935,9 @@
       <c r="F239" t="s">
         <v>41</v>
       </c>
-      <c r="G239"/>
+      <c r="G239" t="n">
+        <v>2</v>
+      </c>
       <c r="H239" t="b">
         <v>0</v>
       </c>
@@ -8690,7 +8964,9 @@
       <c r="F240" t="s">
         <v>43</v>
       </c>
-      <c r="G240"/>
+      <c r="G240" t="n">
+        <v>2</v>
+      </c>
       <c r="H240" t="b">
         <v>0</v>
       </c>
@@ -8717,7 +8993,9 @@
       <c r="F241" t="s">
         <v>221</v>
       </c>
-      <c r="G241"/>
+      <c r="G241" t="n">
+        <v>2</v>
+      </c>
       <c r="H241" t="b">
         <v>0</v>
       </c>
@@ -8889,7 +9167,9 @@
       <c r="F247" t="s">
         <v>226</v>
       </c>
-      <c r="G247"/>
+      <c r="G247" t="n">
+        <v>2</v>
+      </c>
       <c r="H247" t="b">
         <v>0</v>
       </c>
@@ -8916,7 +9196,9 @@
       <c r="F248" t="s">
         <v>227</v>
       </c>
-      <c r="G248"/>
+      <c r="G248" t="n">
+        <v>2</v>
+      </c>
       <c r="H248" t="b">
         <v>0</v>
       </c>
@@ -8972,7 +9254,9 @@
       <c r="F250" t="s">
         <v>229</v>
       </c>
-      <c r="G250"/>
+      <c r="G250" t="n">
+        <v>2</v>
+      </c>
       <c r="H250" t="b">
         <v>0</v>
       </c>
@@ -8999,7 +9283,9 @@
       <c r="F251" t="s">
         <v>230</v>
       </c>
-      <c r="G251"/>
+      <c r="G251" t="n">
+        <v>2</v>
+      </c>
       <c r="H251" t="b">
         <v>0</v>
       </c>
@@ -9026,7 +9312,9 @@
       <c r="F252" t="s">
         <v>36</v>
       </c>
-      <c r="G252"/>
+      <c r="G252" t="n">
+        <v>2</v>
+      </c>
       <c r="H252" t="b">
         <v>0</v>
       </c>
@@ -9053,7 +9341,9 @@
       <c r="F253" t="s">
         <v>39</v>
       </c>
-      <c r="G253"/>
+      <c r="G253" t="n">
+        <v>2</v>
+      </c>
       <c r="H253" t="b">
         <v>0</v>
       </c>
@@ -9080,7 +9370,9 @@
       <c r="F254" t="s">
         <v>41</v>
       </c>
-      <c r="G254"/>
+      <c r="G254" t="n">
+        <v>2</v>
+      </c>
       <c r="H254" t="b">
         <v>0</v>
       </c>
@@ -9107,7 +9399,9 @@
       <c r="F255" t="s">
         <v>43</v>
       </c>
-      <c r="G255"/>
+      <c r="G255" t="n">
+        <v>2</v>
+      </c>
       <c r="H255" t="b">
         <v>0</v>
       </c>
@@ -9163,7 +9457,9 @@
       <c r="F257" t="s">
         <v>233</v>
       </c>
-      <c r="G257"/>
+      <c r="G257" t="n">
+        <v>2</v>
+      </c>
       <c r="H257" t="b">
         <v>0</v>
       </c>
@@ -9190,7 +9486,9 @@
       <c r="F258" t="s">
         <v>234</v>
       </c>
-      <c r="G258"/>
+      <c r="G258" t="n">
+        <v>2</v>
+      </c>
       <c r="H258" t="b">
         <v>0</v>
       </c>
@@ -9304,7 +9602,9 @@
       <c r="F262" t="s">
         <v>236</v>
       </c>
-      <c r="G262"/>
+      <c r="G262" t="n">
+        <v>2</v>
+      </c>
       <c r="H262" t="b">
         <v>0</v>
       </c>
@@ -9331,7 +9631,9 @@
       <c r="F263" t="s">
         <v>237</v>
       </c>
-      <c r="G263"/>
+      <c r="G263" t="n">
+        <v>3</v>
+      </c>
       <c r="H263" t="b">
         <v>1</v>
       </c>
@@ -9387,7 +9689,9 @@
       <c r="F265" t="s">
         <v>239</v>
       </c>
-      <c r="G265"/>
+      <c r="G265" t="n">
+        <v>2</v>
+      </c>
       <c r="H265" t="b">
         <v>0</v>
       </c>
@@ -9414,7 +9718,9 @@
       <c r="F266" t="s">
         <v>240</v>
       </c>
-      <c r="G266"/>
+      <c r="G266" t="n">
+        <v>2</v>
+      </c>
       <c r="H266" t="b">
         <v>0</v>
       </c>
@@ -9441,7 +9747,9 @@
       <c r="F267" t="s">
         <v>36</v>
       </c>
-      <c r="G267"/>
+      <c r="G267" t="n">
+        <v>2</v>
+      </c>
       <c r="H267" t="b">
         <v>0</v>
       </c>
@@ -9555,7 +9863,9 @@
       <c r="F271" t="s">
         <v>244</v>
       </c>
-      <c r="G271"/>
+      <c r="G271" t="n">
+        <v>2</v>
+      </c>
       <c r="H271" t="b">
         <v>0</v>
       </c>
@@ -9582,7 +9892,9 @@
       <c r="F272" t="s">
         <v>246</v>
       </c>
-      <c r="G272"/>
+      <c r="G272" t="n">
+        <v>2</v>
+      </c>
       <c r="H272" t="b">
         <v>0</v>
       </c>
@@ -9609,7 +9921,9 @@
       <c r="F273" t="s">
         <v>247</v>
       </c>
-      <c r="G273"/>
+      <c r="G273" t="n">
+        <v>2</v>
+      </c>
       <c r="H273" t="b">
         <v>0</v>
       </c>
@@ -9723,7 +10037,9 @@
       <c r="F277" t="s">
         <v>249</v>
       </c>
-      <c r="G277"/>
+      <c r="G277" t="n">
+        <v>2</v>
+      </c>
       <c r="H277" t="b">
         <v>0</v>
       </c>
@@ -9750,7 +10066,9 @@
       <c r="F278" t="s">
         <v>250</v>
       </c>
-      <c r="G278"/>
+      <c r="G278" t="n">
+        <v>3</v>
+      </c>
       <c r="H278" t="b">
         <v>1</v>
       </c>
@@ -9806,7 +10124,9 @@
       <c r="F280" t="s">
         <v>252</v>
       </c>
-      <c r="G280"/>
+      <c r="G280" t="n">
+        <v>2</v>
+      </c>
       <c r="H280" t="b">
         <v>0</v>
       </c>
@@ -9833,7 +10153,9 @@
       <c r="F281" t="s">
         <v>253</v>
       </c>
-      <c r="G281"/>
+      <c r="G281" t="n">
+        <v>2</v>
+      </c>
       <c r="H281" t="b">
         <v>0</v>
       </c>
@@ -9860,7 +10182,9 @@
       <c r="F282" t="s">
         <v>36</v>
       </c>
-      <c r="G282"/>
+      <c r="G282" t="n">
+        <v>2</v>
+      </c>
       <c r="H282" t="b">
         <v>0</v>
       </c>
@@ -9974,7 +10298,9 @@
       <c r="F286" t="s">
         <v>257</v>
       </c>
-      <c r="G286"/>
+      <c r="G286" t="n">
+        <v>2</v>
+      </c>
       <c r="H286" t="b">
         <v>0</v>
       </c>
@@ -10146,7 +10472,9 @@
       <c r="F292" t="s">
         <v>263</v>
       </c>
-      <c r="G292"/>
+      <c r="G292" t="n">
+        <v>2</v>
+      </c>
       <c r="H292" t="b">
         <v>0</v>
       </c>
@@ -10173,7 +10501,9 @@
       <c r="F293" t="s">
         <v>264</v>
       </c>
-      <c r="G293"/>
+      <c r="G293" t="n">
+        <v>2</v>
+      </c>
       <c r="H293" t="b">
         <v>0</v>
       </c>
@@ -10229,7 +10559,9 @@
       <c r="F295" t="s">
         <v>266</v>
       </c>
-      <c r="G295"/>
+      <c r="G295" t="n">
+        <v>2</v>
+      </c>
       <c r="H295" t="b">
         <v>0</v>
       </c>
@@ -10256,7 +10588,9 @@
       <c r="F296" t="s">
         <v>267</v>
       </c>
-      <c r="G296"/>
+      <c r="G296" t="n">
+        <v>2</v>
+      </c>
       <c r="H296" t="b">
         <v>0</v>
       </c>
@@ -10283,7 +10617,9 @@
       <c r="F297" t="s">
         <v>36</v>
       </c>
-      <c r="G297"/>
+      <c r="G297" t="n">
+        <v>2</v>
+      </c>
       <c r="H297" t="b">
         <v>0</v>
       </c>
@@ -10397,7 +10733,9 @@
       <c r="F301" t="s">
         <v>271</v>
       </c>
-      <c r="G301"/>
+      <c r="G301" t="n">
+        <v>2</v>
+      </c>
       <c r="H301" t="b">
         <v>0</v>
       </c>
@@ -10569,7 +10907,9 @@
       <c r="F307" t="s">
         <v>276</v>
       </c>
-      <c r="G307"/>
+      <c r="G307" t="n">
+        <v>2</v>
+      </c>
       <c r="H307" t="b">
         <v>0</v>
       </c>
@@ -10596,7 +10936,9 @@
       <c r="F308" t="s">
         <v>277</v>
       </c>
-      <c r="G308"/>
+      <c r="G308" t="n">
+        <v>2</v>
+      </c>
       <c r="H308" t="b">
         <v>0</v>
       </c>
@@ -10652,7 +10994,9 @@
       <c r="F310" t="s">
         <v>279</v>
       </c>
-      <c r="G310"/>
+      <c r="G310" t="n">
+        <v>2</v>
+      </c>
       <c r="H310" t="b">
         <v>0</v>
       </c>
@@ -10679,7 +11023,9 @@
       <c r="F311" t="s">
         <v>280</v>
       </c>
-      <c r="G311"/>
+      <c r="G311" t="n">
+        <v>2</v>
+      </c>
       <c r="H311" t="b">
         <v>0</v>
       </c>
@@ -10706,7 +11052,9 @@
       <c r="F312" t="s">
         <v>36</v>
       </c>
-      <c r="G312"/>
+      <c r="G312" t="n">
+        <v>2</v>
+      </c>
       <c r="H312" t="b">
         <v>0</v>
       </c>
@@ -10820,7 +11168,9 @@
       <c r="F316" t="s">
         <v>284</v>
       </c>
-      <c r="G316"/>
+      <c r="G316" t="n">
+        <v>2</v>
+      </c>
       <c r="H316" t="b">
         <v>0</v>
       </c>
@@ -10992,7 +11342,9 @@
       <c r="F322" t="s">
         <v>289</v>
       </c>
-      <c r="G322"/>
+      <c r="G322" t="n">
+        <v>2</v>
+      </c>
       <c r="H322" t="b">
         <v>0</v>
       </c>
@@ -11019,7 +11371,9 @@
       <c r="F323" t="s">
         <v>290</v>
       </c>
-      <c r="G323"/>
+      <c r="G323" t="n">
+        <v>2</v>
+      </c>
       <c r="H323" t="b">
         <v>0</v>
       </c>
@@ -11075,7 +11429,9 @@
       <c r="F325" t="s">
         <v>292</v>
       </c>
-      <c r="G325"/>
+      <c r="G325" t="n">
+        <v>3</v>
+      </c>
       <c r="H325" t="b">
         <v>1</v>
       </c>
@@ -11102,7 +11458,9 @@
       <c r="F326" t="s">
         <v>293</v>
       </c>
-      <c r="G326"/>
+      <c r="G326" t="n">
+        <v>2</v>
+      </c>
       <c r="H326" t="b">
         <v>0</v>
       </c>
@@ -11129,7 +11487,9 @@
       <c r="F327" t="s">
         <v>36</v>
       </c>
-      <c r="G327"/>
+      <c r="G327" t="n">
+        <v>2</v>
+      </c>
       <c r="H327" t="b">
         <v>0</v>
       </c>
@@ -11156,7 +11516,9 @@
       <c r="F328" t="s">
         <v>294</v>
       </c>
-      <c r="G328"/>
+      <c r="G328" t="n">
+        <v>2</v>
+      </c>
       <c r="H328" t="b">
         <v>0</v>
       </c>
@@ -11212,7 +11574,9 @@
       <c r="F330" t="s">
         <v>296</v>
       </c>
-      <c r="G330"/>
+      <c r="G330" t="n">
+        <v>2</v>
+      </c>
       <c r="H330" t="b">
         <v>0</v>
       </c>
@@ -11239,7 +11603,9 @@
       <c r="F331" t="s">
         <v>297</v>
       </c>
-      <c r="G331"/>
+      <c r="G331" t="n">
+        <v>2</v>
+      </c>
       <c r="H331" t="b">
         <v>0</v>
       </c>
@@ -11266,7 +11632,9 @@
       <c r="F332" t="s">
         <v>299</v>
       </c>
-      <c r="G332"/>
+      <c r="G332" t="n">
+        <v>2</v>
+      </c>
       <c r="H332" t="b">
         <v>0</v>
       </c>
@@ -11409,7 +11777,9 @@
       <c r="F337" t="s">
         <v>303</v>
       </c>
-      <c r="G337"/>
+      <c r="G337" t="n">
+        <v>2</v>
+      </c>
       <c r="H337" t="b">
         <v>0</v>
       </c>
@@ -11436,7 +11806,9 @@
       <c r="F338" t="s">
         <v>304</v>
       </c>
-      <c r="G338"/>
+      <c r="G338" t="n">
+        <v>2</v>
+      </c>
       <c r="H338" t="b">
         <v>0</v>
       </c>
@@ -11492,7 +11864,9 @@
       <c r="F340" t="s">
         <v>306</v>
       </c>
-      <c r="G340"/>
+      <c r="G340" t="n">
+        <v>3</v>
+      </c>
       <c r="H340" t="b">
         <v>1</v>
       </c>
@@ -11548,7 +11922,9 @@
       <c r="F342" t="s">
         <v>36</v>
       </c>
-      <c r="G342"/>
+      <c r="G342" t="n">
+        <v>2</v>
+      </c>
       <c r="H342" t="b">
         <v>0</v>
       </c>
@@ -11575,7 +11951,9 @@
       <c r="F343" t="s">
         <v>39</v>
       </c>
-      <c r="G343"/>
+      <c r="G343" t="n">
+        <v>2</v>
+      </c>
       <c r="H343" t="b">
         <v>0</v>
       </c>
@@ -11602,7 +11980,9 @@
       <c r="F344" t="s">
         <v>41</v>
       </c>
-      <c r="G344"/>
+      <c r="G344" t="n">
+        <v>2</v>
+      </c>
       <c r="H344" t="b">
         <v>0</v>
       </c>
@@ -11629,7 +12009,9 @@
       <c r="F345" t="s">
         <v>43</v>
       </c>
-      <c r="G345"/>
+      <c r="G345" t="n">
+        <v>2</v>
+      </c>
       <c r="H345" t="b">
         <v>0</v>
       </c>
@@ -11656,7 +12038,9 @@
       <c r="F346" t="s">
         <v>308</v>
       </c>
-      <c r="G346"/>
+      <c r="G346" t="n">
+        <v>2</v>
+      </c>
       <c r="H346" t="b">
         <v>0</v>
       </c>
@@ -11828,7 +12212,9 @@
       <c r="F352" t="s">
         <v>314</v>
       </c>
-      <c r="G352"/>
+      <c r="G352" t="n">
+        <v>3</v>
+      </c>
       <c r="H352" t="b">
         <v>1</v>
       </c>
@@ -11855,7 +12241,9 @@
       <c r="F353" t="s">
         <v>315</v>
       </c>
-      <c r="G353"/>
+      <c r="G353" t="n">
+        <v>2</v>
+      </c>
       <c r="H353" t="b">
         <v>0</v>
       </c>
@@ -11911,7 +12299,9 @@
       <c r="F355" t="s">
         <v>317</v>
       </c>
-      <c r="G355"/>
+      <c r="G355" t="n">
+        <v>2</v>
+      </c>
       <c r="H355" t="b">
         <v>0</v>
       </c>
@@ -11938,7 +12328,9 @@
       <c r="F356" t="s">
         <v>318</v>
       </c>
-      <c r="G356"/>
+      <c r="G356" t="n">
+        <v>2</v>
+      </c>
       <c r="H356" t="b">
         <v>0</v>
       </c>
@@ -11965,7 +12357,9 @@
       <c r="F357" t="s">
         <v>36</v>
       </c>
-      <c r="G357"/>
+      <c r="G357" t="n">
+        <v>2</v>
+      </c>
       <c r="H357" t="b">
         <v>0</v>
       </c>
@@ -12050,7 +12444,9 @@
       <c r="F360" t="s">
         <v>321</v>
       </c>
-      <c r="G360"/>
+      <c r="G360" t="n">
+        <v>2</v>
+      </c>
       <c r="H360" t="b">
         <v>0</v>
       </c>
@@ -12106,7 +12502,9 @@
       <c r="F362" t="s">
         <v>324</v>
       </c>
-      <c r="G362"/>
+      <c r="G362" t="n">
+        <v>2</v>
+      </c>
       <c r="H362" t="b">
         <v>0</v>
       </c>
@@ -12249,7 +12647,9 @@
       <c r="F367" t="s">
         <v>328</v>
       </c>
-      <c r="G367"/>
+      <c r="G367" t="n">
+        <v>2</v>
+      </c>
       <c r="H367" t="b">
         <v>0</v>
       </c>
@@ -12276,7 +12676,9 @@
       <c r="F368" t="s">
         <v>329</v>
       </c>
-      <c r="G368"/>
+      <c r="G368" t="n">
+        <v>2</v>
+      </c>
       <c r="H368" t="b">
         <v>0</v>
       </c>
@@ -12332,7 +12734,9 @@
       <c r="F370" t="s">
         <v>331</v>
       </c>
-      <c r="G370"/>
+      <c r="G370" t="n">
+        <v>3</v>
+      </c>
       <c r="H370" t="b">
         <v>1</v>
       </c>
@@ -12359,7 +12763,9 @@
       <c r="F371" t="s">
         <v>332</v>
       </c>
-      <c r="G371"/>
+      <c r="G371" t="n">
+        <v>2</v>
+      </c>
       <c r="H371" t="b">
         <v>0</v>
       </c>
@@ -12386,7 +12792,9 @@
       <c r="F372" t="s">
         <v>36</v>
       </c>
-      <c r="G372"/>
+      <c r="G372" t="n">
+        <v>2</v>
+      </c>
       <c r="H372" t="b">
         <v>0</v>
       </c>
@@ -12413,7 +12821,9 @@
       <c r="F373" t="s">
         <v>39</v>
       </c>
-      <c r="G373"/>
+      <c r="G373" t="n">
+        <v>2</v>
+      </c>
       <c r="H373" t="b">
         <v>0</v>
       </c>
@@ -12440,7 +12850,9 @@
       <c r="F374" t="s">
         <v>41</v>
       </c>
-      <c r="G374"/>
+      <c r="G374" t="n">
+        <v>2</v>
+      </c>
       <c r="H374" t="b">
         <v>0</v>
       </c>
@@ -12467,7 +12879,9 @@
       <c r="F375" t="s">
         <v>43</v>
       </c>
-      <c r="G375"/>
+      <c r="G375" t="n">
+        <v>2</v>
+      </c>
       <c r="H375" t="b">
         <v>0</v>
       </c>
@@ -12494,7 +12908,9 @@
       <c r="F376" t="s">
         <v>333</v>
       </c>
-      <c r="G376"/>
+      <c r="G376" t="n">
+        <v>2</v>
+      </c>
       <c r="H376" t="b">
         <v>0</v>
       </c>
@@ -12666,7 +13082,9 @@
       <c r="F382" t="s">
         <v>338</v>
       </c>
-      <c r="G382"/>
+      <c r="G382" t="n">
+        <v>2</v>
+      </c>
       <c r="H382" t="b">
         <v>0</v>
       </c>
@@ -12693,7 +13111,9 @@
       <c r="F383" t="s">
         <v>339</v>
       </c>
-      <c r="G383"/>
+      <c r="G383" t="n">
+        <v>2</v>
+      </c>
       <c r="H383" t="b">
         <v>0</v>
       </c>
@@ -12749,7 +13169,9 @@
       <c r="F385" t="s">
         <v>341</v>
       </c>
-      <c r="G385"/>
+      <c r="G385" t="n">
+        <v>3</v>
+      </c>
       <c r="H385" t="b">
         <v>1</v>
       </c>
@@ -12776,7 +13198,9 @@
       <c r="F386" t="s">
         <v>342</v>
       </c>
-      <c r="G386"/>
+      <c r="G386" t="n">
+        <v>2</v>
+      </c>
       <c r="H386" t="b">
         <v>0</v>
       </c>
@@ -12803,7 +13227,9 @@
       <c r="F387" t="s">
         <v>36</v>
       </c>
-      <c r="G387"/>
+      <c r="G387" t="n">
+        <v>2</v>
+      </c>
       <c r="H387" t="b">
         <v>0</v>
       </c>
@@ -12830,7 +13256,9 @@
       <c r="F388" t="s">
         <v>343</v>
       </c>
-      <c r="G388"/>
+      <c r="G388" t="n">
+        <v>2</v>
+      </c>
       <c r="H388" t="b">
         <v>0</v>
       </c>
@@ -12857,7 +13285,9 @@
       <c r="F389" t="s">
         <v>344</v>
       </c>
-      <c r="G389"/>
+      <c r="G389" t="n">
+        <v>2</v>
+      </c>
       <c r="H389" t="b">
         <v>0</v>
       </c>
@@ -12884,7 +13314,9 @@
       <c r="F390" t="s">
         <v>345</v>
       </c>
-      <c r="G390"/>
+      <c r="G390" t="n">
+        <v>2</v>
+      </c>
       <c r="H390" t="b">
         <v>0</v>
       </c>
@@ -12911,7 +13343,9 @@
       <c r="F391" t="s">
         <v>346</v>
       </c>
-      <c r="G391"/>
+      <c r="G391" t="n">
+        <v>2</v>
+      </c>
       <c r="H391" t="b">
         <v>0</v>
       </c>
@@ -13083,7 +13517,9 @@
       <c r="F397" t="s">
         <v>352</v>
       </c>
-      <c r="G397"/>
+      <c r="G397" t="n">
+        <v>2</v>
+      </c>
       <c r="H397" t="b">
         <v>0</v>
       </c>
@@ -13110,7 +13546,9 @@
       <c r="F398" t="s">
         <v>353</v>
       </c>
-      <c r="G398"/>
+      <c r="G398" t="n">
+        <v>2</v>
+      </c>
       <c r="H398" t="b">
         <v>0</v>
       </c>
@@ -13166,7 +13604,9 @@
       <c r="F400" t="s">
         <v>355</v>
       </c>
-      <c r="G400"/>
+      <c r="G400" t="n">
+        <v>2</v>
+      </c>
       <c r="H400" t="b">
         <v>0</v>
       </c>
@@ -13193,7 +13633,9 @@
       <c r="F401" t="s">
         <v>356</v>
       </c>
-      <c r="G401"/>
+      <c r="G401" t="n">
+        <v>2</v>
+      </c>
       <c r="H401" t="b">
         <v>0</v>
       </c>
@@ -13220,7 +13662,9 @@
       <c r="F402" t="s">
         <v>36</v>
       </c>
-      <c r="G402"/>
+      <c r="G402" t="n">
+        <v>2</v>
+      </c>
       <c r="H402" t="b">
         <v>0</v>
       </c>
@@ -13247,7 +13691,9 @@
       <c r="F403" t="s">
         <v>39</v>
       </c>
-      <c r="G403"/>
+      <c r="G403" t="n">
+        <v>2</v>
+      </c>
       <c r="H403" t="b">
         <v>0</v>
       </c>
@@ -13274,7 +13720,9 @@
       <c r="F404" t="s">
         <v>41</v>
       </c>
-      <c r="G404"/>
+      <c r="G404" t="n">
+        <v>2</v>
+      </c>
       <c r="H404" t="b">
         <v>0</v>
       </c>
@@ -13301,7 +13749,9 @@
       <c r="F405" t="s">
         <v>43</v>
       </c>
-      <c r="G405"/>
+      <c r="G405" t="n">
+        <v>2</v>
+      </c>
       <c r="H405" t="b">
         <v>0</v>
       </c>
@@ -13328,7 +13778,9 @@
       <c r="F406" t="s">
         <v>357</v>
       </c>
-      <c r="G406"/>
+      <c r="G406" t="n">
+        <v>2</v>
+      </c>
       <c r="H406" t="b">
         <v>0</v>
       </c>
@@ -13500,7 +13952,9 @@
       <c r="F412" t="s">
         <v>362</v>
       </c>
-      <c r="G412"/>
+      <c r="G412" t="n">
+        <v>2</v>
+      </c>
       <c r="H412" t="b">
         <v>0</v>
       </c>
@@ -13527,7 +13981,9 @@
       <c r="F413" t="s">
         <v>363</v>
       </c>
-      <c r="G413"/>
+      <c r="G413" t="n">
+        <v>2</v>
+      </c>
       <c r="H413" t="b">
         <v>0</v>
       </c>
@@ -13583,7 +14039,9 @@
       <c r="F415" t="s">
         <v>365</v>
       </c>
-      <c r="G415"/>
+      <c r="G415" t="n">
+        <v>2</v>
+      </c>
       <c r="H415" t="b">
         <v>0</v>
       </c>
@@ -13610,7 +14068,9 @@
       <c r="F416" t="s">
         <v>366</v>
       </c>
-      <c r="G416"/>
+      <c r="G416" t="n">
+        <v>2</v>
+      </c>
       <c r="H416" t="b">
         <v>0</v>
       </c>
@@ -13637,7 +14097,9 @@
       <c r="F417" t="s">
         <v>36</v>
       </c>
-      <c r="G417"/>
+      <c r="G417" t="n">
+        <v>2</v>
+      </c>
       <c r="H417" t="b">
         <v>0</v>
       </c>
@@ -13664,7 +14126,9 @@
       <c r="F418" t="s">
         <v>367</v>
       </c>
-      <c r="G418"/>
+      <c r="G418" t="n">
+        <v>2</v>
+      </c>
       <c r="H418" t="b">
         <v>0</v>
       </c>
@@ -13691,7 +14155,9 @@
       <c r="F419" t="s">
         <v>368</v>
       </c>
-      <c r="G419"/>
+      <c r="G419" t="n">
+        <v>2</v>
+      </c>
       <c r="H419" t="b">
         <v>0</v>
       </c>
@@ -13718,7 +14184,9 @@
       <c r="F420" t="s">
         <v>369</v>
       </c>
-      <c r="G420"/>
+      <c r="G420" t="n">
+        <v>2</v>
+      </c>
       <c r="H420" t="b">
         <v>0</v>
       </c>
@@ -13745,7 +14213,9 @@
       <c r="F421" t="s">
         <v>370</v>
       </c>
-      <c r="G421"/>
+      <c r="G421" t="n">
+        <v>2</v>
+      </c>
       <c r="H421" t="b">
         <v>0</v>
       </c>
@@ -13772,7 +14242,9 @@
       <c r="F422" t="s">
         <v>372</v>
       </c>
-      <c r="G422"/>
+      <c r="G422" t="n">
+        <v>2</v>
+      </c>
       <c r="H422" t="b">
         <v>0</v>
       </c>
@@ -13799,7 +14271,9 @@
       <c r="F423" t="s">
         <v>373</v>
       </c>
-      <c r="G423"/>
+      <c r="G423" t="n">
+        <v>2</v>
+      </c>
       <c r="H423" t="b">
         <v>0</v>
       </c>
@@ -13913,7 +14387,9 @@
       <c r="F427" t="s">
         <v>376</v>
       </c>
-      <c r="G427"/>
+      <c r="G427" t="n">
+        <v>2</v>
+      </c>
       <c r="H427" t="b">
         <v>0</v>
       </c>
@@ -13940,7 +14416,9 @@
       <c r="F428" t="s">
         <v>377</v>
       </c>
-      <c r="G428"/>
+      <c r="G428" t="n">
+        <v>2</v>
+      </c>
       <c r="H428" t="b">
         <v>0</v>
       </c>
@@ -13996,7 +14474,9 @@
       <c r="F430" t="s">
         <v>379</v>
       </c>
-      <c r="G430"/>
+      <c r="G430" t="n">
+        <v>2</v>
+      </c>
       <c r="H430" t="b">
         <v>0</v>
       </c>
@@ -14023,7 +14503,9 @@
       <c r="F431" t="s">
         <v>380</v>
       </c>
-      <c r="G431"/>
+      <c r="G431" t="n">
+        <v>2</v>
+      </c>
       <c r="H431" t="b">
         <v>0</v>
       </c>
@@ -14050,7 +14532,9 @@
       <c r="F432" t="s">
         <v>36</v>
       </c>
-      <c r="G432"/>
+      <c r="G432" t="n">
+        <v>2</v>
+      </c>
       <c r="H432" t="b">
         <v>0</v>
       </c>
@@ -14077,7 +14561,9 @@
       <c r="F433" t="s">
         <v>381</v>
       </c>
-      <c r="G433"/>
+      <c r="G433" t="n">
+        <v>2</v>
+      </c>
       <c r="H433" t="b">
         <v>0</v>
       </c>
@@ -14104,7 +14590,9 @@
       <c r="F434" t="s">
         <v>382</v>
       </c>
-      <c r="G434"/>
+      <c r="G434" t="n">
+        <v>2</v>
+      </c>
       <c r="H434" t="b">
         <v>0</v>
       </c>
@@ -14131,7 +14619,9 @@
       <c r="F435" t="s">
         <v>383</v>
       </c>
-      <c r="G435"/>
+      <c r="G435" t="n">
+        <v>2</v>
+      </c>
       <c r="H435" t="b">
         <v>0</v>
       </c>
@@ -14158,7 +14648,9 @@
       <c r="F436" t="s">
         <v>384</v>
       </c>
-      <c r="G436"/>
+      <c r="G436" t="n">
+        <v>2</v>
+      </c>
       <c r="H436" t="b">
         <v>0</v>
       </c>
@@ -14330,7 +14822,9 @@
       <c r="F442" t="s">
         <v>389</v>
       </c>
-      <c r="G442"/>
+      <c r="G442" t="n">
+        <v>3</v>
+      </c>
       <c r="H442" t="b">
         <v>1</v>
       </c>
@@ -14357,7 +14851,9 @@
       <c r="F443" t="s">
         <v>390</v>
       </c>
-      <c r="G443"/>
+      <c r="G443" t="n">
+        <v>3</v>
+      </c>
       <c r="H443" t="b">
         <v>1</v>
       </c>
@@ -14413,7 +14909,9 @@
       <c r="F445" t="s">
         <v>392</v>
       </c>
-      <c r="G445"/>
+      <c r="G445" t="n">
+        <v>2</v>
+      </c>
       <c r="H445" t="b">
         <v>0</v>
       </c>
@@ -14440,7 +14938,9 @@
       <c r="F446" t="s">
         <v>393</v>
       </c>
-      <c r="G446"/>
+      <c r="G446" t="n">
+        <v>2</v>
+      </c>
       <c r="H446" t="b">
         <v>0</v>
       </c>
@@ -14467,7 +14967,9 @@
       <c r="F447" t="s">
         <v>36</v>
       </c>
-      <c r="G447"/>
+      <c r="G447" t="n">
+        <v>2</v>
+      </c>
       <c r="H447" t="b">
         <v>0</v>
       </c>
@@ -14494,7 +14996,9 @@
       <c r="F448" t="s">
         <v>39</v>
       </c>
-      <c r="G448"/>
+      <c r="G448" t="n">
+        <v>2</v>
+      </c>
       <c r="H448" t="b">
         <v>0</v>
       </c>
@@ -14521,7 +15025,9 @@
       <c r="F449" t="s">
         <v>41</v>
       </c>
-      <c r="G449"/>
+      <c r="G449" t="n">
+        <v>2</v>
+      </c>
       <c r="H449" t="b">
         <v>0</v>
       </c>
@@ -14548,7 +15054,9 @@
       <c r="F450" t="s">
         <v>394</v>
       </c>
-      <c r="G450"/>
+      <c r="G450" t="n">
+        <v>2</v>
+      </c>
       <c r="H450" t="b">
         <v>0</v>
       </c>
@@ -14604,7 +15112,9 @@
       <c r="F452" t="s">
         <v>397</v>
       </c>
-      <c r="G452"/>
+      <c r="G452" t="n">
+        <v>2</v>
+      </c>
       <c r="H452" t="b">
         <v>0</v>
       </c>
@@ -14631,7 +15141,9 @@
       <c r="F453" t="s">
         <v>398</v>
       </c>
-      <c r="G453"/>
+      <c r="G453" t="n">
+        <v>2</v>
+      </c>
       <c r="H453" t="b">
         <v>0</v>
       </c>
@@ -14745,7 +15257,9 @@
       <c r="F457" t="s">
         <v>400</v>
       </c>
-      <c r="G457"/>
+      <c r="G457" t="n">
+        <v>2</v>
+      </c>
       <c r="H457" t="b">
         <v>0</v>
       </c>
@@ -14772,7 +15286,9 @@
       <c r="F458" t="s">
         <v>401</v>
       </c>
-      <c r="G458"/>
+      <c r="G458" t="n">
+        <v>2</v>
+      </c>
       <c r="H458" t="b">
         <v>0</v>
       </c>
@@ -14828,7 +15344,9 @@
       <c r="F460" t="s">
         <v>403</v>
       </c>
-      <c r="G460"/>
+      <c r="G460" t="n">
+        <v>2</v>
+      </c>
       <c r="H460" t="b">
         <v>0</v>
       </c>
@@ -14855,7 +15373,9 @@
       <c r="F461" t="s">
         <v>404</v>
       </c>
-      <c r="G461"/>
+      <c r="G461" t="n">
+        <v>2</v>
+      </c>
       <c r="H461" t="b">
         <v>0</v>
       </c>
@@ -14882,7 +15402,9 @@
       <c r="F462" t="s">
         <v>36</v>
       </c>
-      <c r="G462"/>
+      <c r="G462" t="n">
+        <v>2</v>
+      </c>
       <c r="H462" t="b">
         <v>0</v>
       </c>
@@ -14909,7 +15431,9 @@
       <c r="F463" t="s">
         <v>39</v>
       </c>
-      <c r="G463"/>
+      <c r="G463" t="n">
+        <v>2</v>
+      </c>
       <c r="H463" t="b">
         <v>0</v>
       </c>
@@ -14936,7 +15460,9 @@
       <c r="F464" t="s">
         <v>41</v>
       </c>
-      <c r="G464"/>
+      <c r="G464" t="n">
+        <v>2</v>
+      </c>
       <c r="H464" t="b">
         <v>0</v>
       </c>
@@ -14963,7 +15489,9 @@
       <c r="F465" t="s">
         <v>43</v>
       </c>
-      <c r="G465"/>
+      <c r="G465" t="n">
+        <v>2</v>
+      </c>
       <c r="H465" t="b">
         <v>0</v>
       </c>
@@ -14990,7 +15518,9 @@
       <c r="F466" t="s">
         <v>405</v>
       </c>
-      <c r="G466"/>
+      <c r="G466" t="n">
+        <v>2</v>
+      </c>
       <c r="H466" t="b">
         <v>0</v>
       </c>
@@ -15017,7 +15547,9 @@
       <c r="F467" t="s">
         <v>407</v>
       </c>
-      <c r="G467"/>
+      <c r="G467" t="n">
+        <v>2</v>
+      </c>
       <c r="H467" t="b">
         <v>0</v>
       </c>
@@ -15044,7 +15576,9 @@
       <c r="F468" t="s">
         <v>408</v>
       </c>
-      <c r="G468"/>
+      <c r="G468" t="n">
+        <v>2</v>
+      </c>
       <c r="H468" t="b">
         <v>0</v>
       </c>
@@ -15158,7 +15692,9 @@
       <c r="F472" t="s">
         <v>411</v>
       </c>
-      <c r="G472"/>
+      <c r="G472" t="n">
+        <v>2</v>
+      </c>
       <c r="H472" t="b">
         <v>0</v>
       </c>
@@ -15185,7 +15721,9 @@
       <c r="F473" t="s">
         <v>412</v>
       </c>
-      <c r="G473"/>
+      <c r="G473" t="n">
+        <v>3</v>
+      </c>
       <c r="H473" t="b">
         <v>1</v>
       </c>
@@ -15241,7 +15779,9 @@
       <c r="F475" t="s">
         <v>414</v>
       </c>
-      <c r="G475"/>
+      <c r="G475" t="n">
+        <v>2</v>
+      </c>
       <c r="H475" t="b">
         <v>0</v>
       </c>
@@ -15268,7 +15808,9 @@
       <c r="F476" t="s">
         <v>415</v>
       </c>
-      <c r="G476"/>
+      <c r="G476" t="n">
+        <v>2</v>
+      </c>
       <c r="H476" t="b">
         <v>0</v>
       </c>
@@ -15295,7 +15837,9 @@
       <c r="F477" t="s">
         <v>36</v>
       </c>
-      <c r="G477"/>
+      <c r="G477" t="n">
+        <v>2</v>
+      </c>
       <c r="H477" t="b">
         <v>0</v>
       </c>
@@ -15322,7 +15866,9 @@
       <c r="F478" t="s">
         <v>39</v>
       </c>
-      <c r="G478"/>
+      <c r="G478" t="n">
+        <v>2</v>
+      </c>
       <c r="H478" t="b">
         <v>0</v>
       </c>
@@ -15349,7 +15895,9 @@
       <c r="F479" t="s">
         <v>41</v>
       </c>
-      <c r="G479"/>
+      <c r="G479" t="n">
+        <v>2</v>
+      </c>
       <c r="H479" t="b">
         <v>0</v>
       </c>
@@ -15376,7 +15924,9 @@
       <c r="F480" t="s">
         <v>43</v>
       </c>
-      <c r="G480"/>
+      <c r="G480" t="n">
+        <v>2</v>
+      </c>
       <c r="H480" t="b">
         <v>0</v>
       </c>
@@ -15403,7 +15953,9 @@
       <c r="F481" t="s">
         <v>416</v>
       </c>
-      <c r="G481"/>
+      <c r="G481" t="n">
+        <v>2</v>
+      </c>
       <c r="H481" t="b">
         <v>0</v>
       </c>
@@ -15575,7 +16127,9 @@
       <c r="F487" t="s">
         <v>420</v>
       </c>
-      <c r="G487"/>
+      <c r="G487" t="n">
+        <v>2</v>
+      </c>
       <c r="H487" t="b">
         <v>0</v>
       </c>
@@ -15602,7 +16156,9 @@
       <c r="F488" t="s">
         <v>421</v>
       </c>
-      <c r="G488"/>
+      <c r="G488" t="n">
+        <v>3</v>
+      </c>
       <c r="H488" t="b">
         <v>1</v>
       </c>
@@ -15658,7 +16214,9 @@
       <c r="F490" t="s">
         <v>423</v>
       </c>
-      <c r="G490"/>
+      <c r="G490" t="n">
+        <v>2</v>
+      </c>
       <c r="H490" t="b">
         <v>0</v>
       </c>
@@ -15685,7 +16243,9 @@
       <c r="F491" t="s">
         <v>424</v>
       </c>
-      <c r="G491"/>
+      <c r="G491" t="n">
+        <v>2</v>
+      </c>
       <c r="H491" t="b">
         <v>0</v>
       </c>
@@ -15712,7 +16272,9 @@
       <c r="F492" t="s">
         <v>36</v>
       </c>
-      <c r="G492"/>
+      <c r="G492" t="n">
+        <v>2</v>
+      </c>
       <c r="H492" t="b">
         <v>0</v>
       </c>
@@ -15826,7 +16388,9 @@
       <c r="F496" t="s">
         <v>428</v>
       </c>
-      <c r="G496"/>
+      <c r="G496" t="n">
+        <v>2</v>
+      </c>
       <c r="H496" t="b">
         <v>0</v>
       </c>
@@ -15998,7 +16562,9 @@
       <c r="F502" t="s">
         <v>433</v>
       </c>
-      <c r="G502"/>
+      <c r="G502" t="n">
+        <v>3</v>
+      </c>
       <c r="H502" t="b">
         <v>1</v>
       </c>
@@ -16025,7 +16591,9 @@
       <c r="F503" t="s">
         <v>434</v>
       </c>
-      <c r="G503"/>
+      <c r="G503" t="n">
+        <v>3</v>
+      </c>
       <c r="H503" t="b">
         <v>1</v>
       </c>
@@ -16081,7 +16649,9 @@
       <c r="F505" t="s">
         <v>436</v>
       </c>
-      <c r="G505"/>
+      <c r="G505" t="n">
+        <v>2</v>
+      </c>
       <c r="H505" t="b">
         <v>0</v>
       </c>
@@ -16108,7 +16678,9 @@
       <c r="F506" t="s">
         <v>437</v>
       </c>
-      <c r="G506"/>
+      <c r="G506" t="n">
+        <v>2</v>
+      </c>
       <c r="H506" t="b">
         <v>0</v>
       </c>
@@ -16135,7 +16707,9 @@
       <c r="F507" t="s">
         <v>36</v>
       </c>
-      <c r="G507"/>
+      <c r="G507" t="n">
+        <v>2</v>
+      </c>
       <c r="H507" t="b">
         <v>0</v>
       </c>
@@ -16162,7 +16736,9 @@
       <c r="F508" t="s">
         <v>438</v>
       </c>
-      <c r="G508"/>
+      <c r="G508" t="n">
+        <v>2</v>
+      </c>
       <c r="H508" t="b">
         <v>0</v>
       </c>
@@ -16189,7 +16765,9 @@
       <c r="F509" t="s">
         <v>439</v>
       </c>
-      <c r="G509"/>
+      <c r="G509" t="n">
+        <v>2</v>
+      </c>
       <c r="H509" t="b">
         <v>0</v>
       </c>
@@ -16216,7 +16794,9 @@
       <c r="F510" t="s">
         <v>440</v>
       </c>
-      <c r="G510"/>
+      <c r="G510" t="n">
+        <v>2</v>
+      </c>
       <c r="H510" t="b">
         <v>0</v>
       </c>
@@ -16272,7 +16852,9 @@
       <c r="F512" t="s">
         <v>443</v>
       </c>
-      <c r="G512"/>
+      <c r="G512" t="n">
+        <v>2</v>
+      </c>
       <c r="H512" t="b">
         <v>0</v>
       </c>
@@ -16299,7 +16881,9 @@
       <c r="F513" t="s">
         <v>444</v>
       </c>
-      <c r="G513"/>
+      <c r="G513" t="n">
+        <v>2</v>
+      </c>
       <c r="H513" t="b">
         <v>0</v>
       </c>
@@ -16413,7 +16997,9 @@
       <c r="F517" t="s">
         <v>446</v>
       </c>
-      <c r="G517"/>
+      <c r="G517" t="n">
+        <v>2</v>
+      </c>
       <c r="H517" t="b">
         <v>0</v>
       </c>
@@ -16440,7 +17026,9 @@
       <c r="F518" t="s">
         <v>447</v>
       </c>
-      <c r="G518"/>
+      <c r="G518" t="n">
+        <v>2</v>
+      </c>
       <c r="H518" t="b">
         <v>0</v>
       </c>
@@ -16496,7 +17084,9 @@
       <c r="F520" t="s">
         <v>449</v>
       </c>
-      <c r="G520"/>
+      <c r="G520" t="n">
+        <v>2</v>
+      </c>
       <c r="H520" t="b">
         <v>0</v>
       </c>
@@ -16523,7 +17113,9 @@
       <c r="F521" t="s">
         <v>450</v>
       </c>
-      <c r="G521"/>
+      <c r="G521" t="n">
+        <v>2</v>
+      </c>
       <c r="H521" t="b">
         <v>0</v>
       </c>
@@ -16550,7 +17142,9 @@
       <c r="F522" t="s">
         <v>36</v>
       </c>
-      <c r="G522"/>
+      <c r="G522" t="n">
+        <v>2</v>
+      </c>
       <c r="H522" t="b">
         <v>0</v>
       </c>
@@ -16577,7 +17171,9 @@
       <c r="F523" t="s">
         <v>39</v>
       </c>
-      <c r="G523"/>
+      <c r="G523" t="n">
+        <v>2</v>
+      </c>
       <c r="H523" t="b">
         <v>0</v>
       </c>
@@ -16604,7 +17200,9 @@
       <c r="F524" t="s">
         <v>41</v>
       </c>
-      <c r="G524"/>
+      <c r="G524" t="n">
+        <v>2</v>
+      </c>
       <c r="H524" t="b">
         <v>0</v>
       </c>
@@ -16631,7 +17229,9 @@
       <c r="F525" t="s">
         <v>43</v>
       </c>
-      <c r="G525"/>
+      <c r="G525" t="n">
+        <v>2</v>
+      </c>
       <c r="H525" t="b">
         <v>0</v>
       </c>
@@ -16658,7 +17258,9 @@
       <c r="F526" t="s">
         <v>451</v>
       </c>
-      <c r="G526"/>
+      <c r="G526" t="n">
+        <v>2</v>
+      </c>
       <c r="H526" t="b">
         <v>0</v>
       </c>
@@ -16830,7 +17432,9 @@
       <c r="F532" t="s">
         <v>455</v>
       </c>
-      <c r="G532"/>
+      <c r="G532" t="n">
+        <v>3</v>
+      </c>
       <c r="H532" t="b">
         <v>1</v>
       </c>
@@ -16857,7 +17461,9 @@
       <c r="F533" t="s">
         <v>456</v>
       </c>
-      <c r="G533"/>
+      <c r="G533" t="n">
+        <v>2</v>
+      </c>
       <c r="H533" t="b">
         <v>0</v>
       </c>
@@ -16913,7 +17519,9 @@
       <c r="F535" t="s">
         <v>458</v>
       </c>
-      <c r="G535"/>
+      <c r="G535" t="n">
+        <v>2</v>
+      </c>
       <c r="H535" t="b">
         <v>0</v>
       </c>
@@ -16940,7 +17548,9 @@
       <c r="F536" t="s">
         <v>459</v>
       </c>
-      <c r="G536"/>
+      <c r="G536" t="n">
+        <v>2</v>
+      </c>
       <c r="H536" t="b">
         <v>0</v>
       </c>
@@ -16967,7 +17577,9 @@
       <c r="F537" t="s">
         <v>36</v>
       </c>
-      <c r="G537"/>
+      <c r="G537" t="n">
+        <v>2</v>
+      </c>
       <c r="H537" t="b">
         <v>0</v>
       </c>
@@ -16994,7 +17606,9 @@
       <c r="F538" t="s">
         <v>39</v>
       </c>
-      <c r="G538"/>
+      <c r="G538" t="n">
+        <v>2</v>
+      </c>
       <c r="H538" t="b">
         <v>0</v>
       </c>
@@ -17021,7 +17635,9 @@
       <c r="F539" t="s">
         <v>41</v>
       </c>
-      <c r="G539"/>
+      <c r="G539" t="n">
+        <v>2</v>
+      </c>
       <c r="H539" t="b">
         <v>0</v>
       </c>
@@ -17048,7 +17664,9 @@
       <c r="F540" t="s">
         <v>43</v>
       </c>
-      <c r="G540"/>
+      <c r="G540" t="n">
+        <v>2</v>
+      </c>
       <c r="H540" t="b">
         <v>0</v>
       </c>
@@ -17075,7 +17693,9 @@
       <c r="F541" t="s">
         <v>460</v>
       </c>
-      <c r="G541"/>
+      <c r="G541" t="n">
+        <v>2</v>
+      </c>
       <c r="H541" t="b">
         <v>0</v>
       </c>
@@ -17247,7 +17867,9 @@
       <c r="F547" t="s">
         <v>464</v>
       </c>
-      <c r="G547"/>
+      <c r="G547" t="n">
+        <v>3</v>
+      </c>
       <c r="H547" t="b">
         <v>1</v>
       </c>
@@ -17274,7 +17896,9 @@
       <c r="F548" t="s">
         <v>465</v>
       </c>
-      <c r="G548"/>
+      <c r="G548" t="n">
+        <v>2</v>
+      </c>
       <c r="H548" t="b">
         <v>0</v>
       </c>
@@ -17330,7 +17954,9 @@
       <c r="F550" t="s">
         <v>467</v>
       </c>
-      <c r="G550"/>
+      <c r="G550" t="n">
+        <v>2</v>
+      </c>
       <c r="H550" t="b">
         <v>0</v>
       </c>
@@ -17357,7 +17983,9 @@
       <c r="F551" t="s">
         <v>468</v>
       </c>
-      <c r="G551"/>
+      <c r="G551" t="n">
+        <v>2</v>
+      </c>
       <c r="H551" t="b">
         <v>0</v>
       </c>
@@ -17384,7 +18012,9 @@
       <c r="F552" t="s">
         <v>36</v>
       </c>
-      <c r="G552"/>
+      <c r="G552" t="n">
+        <v>2</v>
+      </c>
       <c r="H552" t="b">
         <v>0</v>
       </c>
@@ -17411,7 +18041,9 @@
       <c r="F553" t="s">
         <v>39</v>
       </c>
-      <c r="G553"/>
+      <c r="G553" t="n">
+        <v>2</v>
+      </c>
       <c r="H553" t="b">
         <v>0</v>
       </c>
@@ -17438,7 +18070,9 @@
       <c r="F554" t="s">
         <v>41</v>
       </c>
-      <c r="G554"/>
+      <c r="G554" t="n">
+        <v>2</v>
+      </c>
       <c r="H554" t="b">
         <v>0</v>
       </c>
@@ -17465,7 +18099,9 @@
       <c r="F555" t="s">
         <v>43</v>
       </c>
-      <c r="G555"/>
+      <c r="G555" t="n">
+        <v>2</v>
+      </c>
       <c r="H555" t="b">
         <v>0</v>
       </c>
@@ -17492,7 +18128,9 @@
       <c r="F556" t="s">
         <v>469</v>
       </c>
-      <c r="G556"/>
+      <c r="G556" t="n">
+        <v>2</v>
+      </c>
       <c r="H556" t="b">
         <v>0</v>
       </c>
@@ -17664,7 +18302,9 @@
       <c r="F562" t="s">
         <v>474</v>
       </c>
-      <c r="G562"/>
+      <c r="G562" t="n">
+        <v>2</v>
+      </c>
       <c r="H562" t="b">
         <v>0</v>
       </c>
@@ -17691,7 +18331,9 @@
       <c r="F563" t="s">
         <v>475</v>
       </c>
-      <c r="G563"/>
+      <c r="G563" t="n">
+        <v>2</v>
+      </c>
       <c r="H563" t="b">
         <v>0</v>
       </c>
@@ -17747,7 +18389,9 @@
       <c r="F565" t="s">
         <v>477</v>
       </c>
-      <c r="G565"/>
+      <c r="G565" t="n">
+        <v>2</v>
+      </c>
       <c r="H565" t="b">
         <v>0</v>
       </c>
@@ -17774,7 +18418,9 @@
       <c r="F566" t="s">
         <v>478</v>
       </c>
-      <c r="G566"/>
+      <c r="G566" t="n">
+        <v>2</v>
+      </c>
       <c r="H566" t="b">
         <v>0</v>
       </c>
@@ -17801,7 +18447,9 @@
       <c r="F567" t="s">
         <v>36</v>
       </c>
-      <c r="G567"/>
+      <c r="G567" t="n">
+        <v>2</v>
+      </c>
       <c r="H567" t="b">
         <v>0</v>
       </c>
@@ -17828,7 +18476,9 @@
       <c r="F568" t="s">
         <v>39</v>
       </c>
-      <c r="G568"/>
+      <c r="G568" t="n">
+        <v>2</v>
+      </c>
       <c r="H568" t="b">
         <v>0</v>
       </c>
@@ -17855,7 +18505,9 @@
       <c r="F569" t="s">
         <v>41</v>
       </c>
-      <c r="G569"/>
+      <c r="G569" t="n">
+        <v>2</v>
+      </c>
       <c r="H569" t="b">
         <v>0</v>
       </c>
@@ -17882,7 +18534,9 @@
       <c r="F570" t="s">
         <v>43</v>
       </c>
-      <c r="G570"/>
+      <c r="G570" t="n">
+        <v>2</v>
+      </c>
       <c r="H570" t="b">
         <v>0</v>
       </c>
@@ -17909,7 +18563,9 @@
       <c r="F571" t="s">
         <v>479</v>
       </c>
-      <c r="G571"/>
+      <c r="G571" t="n">
+        <v>2</v>
+      </c>
       <c r="H571" t="b">
         <v>0</v>
       </c>
@@ -18081,7 +18737,9 @@
       <c r="F577" t="s">
         <v>484</v>
       </c>
-      <c r="G577"/>
+      <c r="G577" t="n">
+        <v>2</v>
+      </c>
       <c r="H577" t="b">
         <v>0</v>
       </c>
@@ -18108,7 +18766,9 @@
       <c r="F578" t="s">
         <v>485</v>
       </c>
-      <c r="G578"/>
+      <c r="G578" t="n">
+        <v>2</v>
+      </c>
       <c r="H578" t="b">
         <v>0</v>
       </c>
@@ -18164,7 +18824,9 @@
       <c r="F580" t="s">
         <v>487</v>
       </c>
-      <c r="G580"/>
+      <c r="G580" t="n">
+        <v>2</v>
+      </c>
       <c r="H580" t="b">
         <v>0</v>
       </c>
@@ -18191,7 +18853,9 @@
       <c r="F581" t="s">
         <v>488</v>
       </c>
-      <c r="G581"/>
+      <c r="G581" t="n">
+        <v>2</v>
+      </c>
       <c r="H581" t="b">
         <v>0</v>
       </c>
@@ -18218,7 +18882,9 @@
       <c r="F582" t="s">
         <v>36</v>
       </c>
-      <c r="G582"/>
+      <c r="G582" t="n">
+        <v>2</v>
+      </c>
       <c r="H582" t="b">
         <v>0</v>
       </c>
@@ -18245,7 +18911,9 @@
       <c r="F583" t="s">
         <v>39</v>
       </c>
-      <c r="G583"/>
+      <c r="G583" t="n">
+        <v>2</v>
+      </c>
       <c r="H583" t="b">
         <v>0</v>
       </c>
@@ -18272,7 +18940,9 @@
       <c r="F584" t="s">
         <v>41</v>
       </c>
-      <c r="G584"/>
+      <c r="G584" t="n">
+        <v>2</v>
+      </c>
       <c r="H584" t="b">
         <v>0</v>
       </c>
@@ -18299,7 +18969,9 @@
       <c r="F585" t="s">
         <v>43</v>
       </c>
-      <c r="G585"/>
+      <c r="G585" t="n">
+        <v>2</v>
+      </c>
       <c r="H585" t="b">
         <v>0</v>
       </c>
@@ -18326,7 +18998,9 @@
       <c r="F586" t="s">
         <v>489</v>
       </c>
-      <c r="G586"/>
+      <c r="G586" t="n">
+        <v>2</v>
+      </c>
       <c r="H586" t="b">
         <v>0</v>
       </c>
@@ -18353,7 +19027,9 @@
       <c r="F587" t="s">
         <v>491</v>
       </c>
-      <c r="G587"/>
+      <c r="G587" t="n">
+        <v>2</v>
+      </c>
       <c r="H587" t="b">
         <v>0</v>
       </c>
@@ -18409,7 +19085,9 @@
       <c r="F589" t="s">
         <v>493</v>
       </c>
-      <c r="G589"/>
+      <c r="G589" t="n">
+        <v>2</v>
+      </c>
       <c r="H589" t="b">
         <v>0</v>
       </c>
@@ -18436,7 +19114,9 @@
       <c r="F590" t="s">
         <v>494</v>
       </c>
-      <c r="G590"/>
+      <c r="G590" t="n">
+        <v>2</v>
+      </c>
       <c r="H590" t="b">
         <v>0</v>
       </c>
@@ -18463,7 +19143,9 @@
       <c r="F591" t="s">
         <v>495</v>
       </c>
-      <c r="G591"/>
+      <c r="G591" t="n">
+        <v>2</v>
+      </c>
       <c r="H591" t="b">
         <v>0</v>
       </c>
@@ -18490,7 +19172,9 @@
       <c r="F592" t="s">
         <v>496</v>
       </c>
-      <c r="G592"/>
+      <c r="G592" t="n">
+        <v>2</v>
+      </c>
       <c r="H592" t="b">
         <v>0</v>
       </c>
@@ -18517,7 +19201,9 @@
       <c r="F593" t="s">
         <v>497</v>
       </c>
-      <c r="G593"/>
+      <c r="G593" t="n">
+        <v>2</v>
+      </c>
       <c r="H593" t="b">
         <v>0</v>
       </c>
@@ -18573,7 +19259,9 @@
       <c r="F595" t="s">
         <v>499</v>
       </c>
-      <c r="G595"/>
+      <c r="G595" t="n">
+        <v>2</v>
+      </c>
       <c r="H595" t="b">
         <v>0</v>
       </c>
@@ -18600,7 +19288,9 @@
       <c r="F596" t="s">
         <v>500</v>
       </c>
-      <c r="G596"/>
+      <c r="G596" t="n">
+        <v>2</v>
+      </c>
       <c r="H596" t="b">
         <v>0</v>
       </c>
@@ -18627,7 +19317,9 @@
       <c r="F597" t="s">
         <v>36</v>
       </c>
-      <c r="G597"/>
+      <c r="G597" t="n">
+        <v>2</v>
+      </c>
       <c r="H597" t="b">
         <v>0</v>
       </c>
@@ -18654,7 +19346,9 @@
       <c r="F598" t="s">
         <v>39</v>
       </c>
-      <c r="G598"/>
+      <c r="G598" t="n">
+        <v>2</v>
+      </c>
       <c r="H598" t="b">
         <v>0</v>
       </c>
@@ -18681,7 +19375,9 @@
       <c r="F599" t="s">
         <v>41</v>
       </c>
-      <c r="G599"/>
+      <c r="G599" t="n">
+        <v>2</v>
+      </c>
       <c r="H599" t="b">
         <v>0</v>
       </c>
@@ -18708,7 +19404,9 @@
       <c r="F600" t="s">
         <v>43</v>
       </c>
-      <c r="G600"/>
+      <c r="G600" t="n">
+        <v>2</v>
+      </c>
       <c r="H600" t="b">
         <v>0</v>
       </c>
@@ -18735,7 +19433,9 @@
       <c r="F601" t="s">
         <v>501</v>
       </c>
-      <c r="G601"/>
+      <c r="G601" t="n">
+        <v>2</v>
+      </c>
       <c r="H601" t="b">
         <v>0</v>
       </c>
@@ -18907,7 +19607,9 @@
       <c r="F607" t="s">
         <v>505</v>
       </c>
-      <c r="G607"/>
+      <c r="G607" t="n">
+        <v>3</v>
+      </c>
       <c r="H607" t="b">
         <v>1</v>
       </c>
@@ -18934,7 +19636,9 @@
       <c r="F608" t="s">
         <v>506</v>
       </c>
-      <c r="G608"/>
+      <c r="G608" t="n">
+        <v>2</v>
+      </c>
       <c r="H608" t="b">
         <v>0</v>
       </c>
@@ -18990,7 +19694,9 @@
       <c r="F610" t="s">
         <v>508</v>
       </c>
-      <c r="G610"/>
+      <c r="G610" t="n">
+        <v>2</v>
+      </c>
       <c r="H610" t="b">
         <v>0</v>
       </c>
@@ -19017,7 +19723,9 @@
       <c r="F611" t="s">
         <v>509</v>
       </c>
-      <c r="G611"/>
+      <c r="G611" t="n">
+        <v>2</v>
+      </c>
       <c r="H611" t="b">
         <v>0</v>
       </c>
@@ -19044,7 +19752,9 @@
       <c r="F612" t="s">
         <v>36</v>
       </c>
-      <c r="G612"/>
+      <c r="G612" t="n">
+        <v>2</v>
+      </c>
       <c r="H612" t="b">
         <v>0</v>
       </c>
@@ -19071,7 +19781,9 @@
       <c r="F613" t="s">
         <v>510</v>
       </c>
-      <c r="G613"/>
+      <c r="G613" t="n">
+        <v>2</v>
+      </c>
       <c r="H613" t="b">
         <v>0</v>
       </c>
@@ -19098,7 +19810,9 @@
       <c r="F614" t="s">
         <v>511</v>
       </c>
-      <c r="G614"/>
+      <c r="G614" t="n">
+        <v>2</v>
+      </c>
       <c r="H614" t="b">
         <v>0</v>
       </c>
@@ -19125,7 +19839,9 @@
       <c r="F615" t="s">
         <v>512</v>
       </c>
-      <c r="G615"/>
+      <c r="G615" t="n">
+        <v>2</v>
+      </c>
       <c r="H615" t="b">
         <v>0</v>
       </c>
@@ -19326,7 +20042,9 @@
       <c r="F622" t="s">
         <v>518</v>
       </c>
-      <c r="G622"/>
+      <c r="G622" t="n">
+        <v>3</v>
+      </c>
       <c r="H622" t="b">
         <v>1</v>
       </c>
@@ -19353,7 +20071,9 @@
       <c r="F623" t="s">
         <v>519</v>
       </c>
-      <c r="G623"/>
+      <c r="G623" t="n">
+        <v>2</v>
+      </c>
       <c r="H623" t="b">
         <v>0</v>
       </c>
@@ -19409,7 +20129,9 @@
       <c r="F625" t="s">
         <v>521</v>
       </c>
-      <c r="G625"/>
+      <c r="G625" t="n">
+        <v>2</v>
+      </c>
       <c r="H625" t="b">
         <v>0</v>
       </c>
@@ -19436,7 +20158,9 @@
       <c r="F626" t="s">
         <v>522</v>
       </c>
-      <c r="G626"/>
+      <c r="G626" t="n">
+        <v>2</v>
+      </c>
       <c r="H626" t="b">
         <v>0</v>
       </c>
@@ -19463,7 +20187,9 @@
       <c r="F627" t="s">
         <v>36</v>
       </c>
-      <c r="G627"/>
+      <c r="G627" t="n">
+        <v>2</v>
+      </c>
       <c r="H627" t="b">
         <v>0</v>
       </c>
@@ -19490,7 +20216,9 @@
       <c r="F628" t="s">
         <v>39</v>
       </c>
-      <c r="G628"/>
+      <c r="G628" t="n">
+        <v>2</v>
+      </c>
       <c r="H628" t="b">
         <v>0</v>
       </c>
@@ -19517,7 +20245,9 @@
       <c r="F629" t="s">
         <v>41</v>
       </c>
-      <c r="G629"/>
+      <c r="G629" t="n">
+        <v>2</v>
+      </c>
       <c r="H629" t="b">
         <v>0</v>
       </c>
@@ -19544,7 +20274,9 @@
       <c r="F630" t="s">
         <v>43</v>
       </c>
-      <c r="G630"/>
+      <c r="G630" t="n">
+        <v>2</v>
+      </c>
       <c r="H630" t="b">
         <v>0</v>
       </c>
@@ -19600,7 +20332,9 @@
       <c r="F632" t="s">
         <v>525</v>
       </c>
-      <c r="G632"/>
+      <c r="G632" t="n">
+        <v>2</v>
+      </c>
       <c r="H632" t="b">
         <v>0</v>
       </c>
@@ -19627,7 +20361,9 @@
       <c r="F633" t="s">
         <v>526</v>
       </c>
-      <c r="G633"/>
+      <c r="G633" t="n">
+        <v>2</v>
+      </c>
       <c r="H633" t="b">
         <v>0</v>
       </c>
@@ -19741,7 +20477,9 @@
       <c r="F637" t="s">
         <v>528</v>
       </c>
-      <c r="G637"/>
+      <c r="G637" t="n">
+        <v>2</v>
+      </c>
       <c r="H637" t="b">
         <v>0</v>
       </c>
@@ -19768,7 +20506,9 @@
       <c r="F638" t="s">
         <v>529</v>
       </c>
-      <c r="G638"/>
+      <c r="G638" t="n">
+        <v>2</v>
+      </c>
       <c r="H638" t="b">
         <v>0</v>
       </c>
@@ -19824,7 +20564,9 @@
       <c r="F640" t="s">
         <v>531</v>
       </c>
-      <c r="G640"/>
+      <c r="G640" t="n">
+        <v>2</v>
+      </c>
       <c r="H640" t="b">
         <v>0</v>
       </c>
@@ -19851,7 +20593,9 @@
       <c r="F641" t="s">
         <v>532</v>
       </c>
-      <c r="G641"/>
+      <c r="G641" t="n">
+        <v>2</v>
+      </c>
       <c r="H641" t="b">
         <v>0</v>
       </c>
@@ -19878,7 +20622,9 @@
       <c r="F642" t="s">
         <v>36</v>
       </c>
-      <c r="G642"/>
+      <c r="G642" t="n">
+        <v>2</v>
+      </c>
       <c r="H642" t="b">
         <v>0</v>
       </c>
@@ -19905,7 +20651,9 @@
       <c r="F643" t="s">
         <v>533</v>
       </c>
-      <c r="G643"/>
+      <c r="G643" t="n">
+        <v>2</v>
+      </c>
       <c r="H643" t="b">
         <v>0</v>
       </c>
@@ -19932,7 +20680,9 @@
       <c r="F644" t="s">
         <v>534</v>
       </c>
-      <c r="G644"/>
+      <c r="G644" t="n">
+        <v>2</v>
+      </c>
       <c r="H644" t="b">
         <v>0</v>
       </c>
@@ -19959,7 +20709,9 @@
       <c r="F645" t="s">
         <v>535</v>
       </c>
-      <c r="G645"/>
+      <c r="G645" t="n">
+        <v>2</v>
+      </c>
       <c r="H645" t="b">
         <v>0</v>
       </c>
@@ -19986,7 +20738,9 @@
       <c r="F646" t="s">
         <v>536</v>
       </c>
-      <c r="G646"/>
+      <c r="G646" t="n">
+        <v>2</v>
+      </c>
       <c r="H646" t="b">
         <v>0</v>
       </c>
@@ -20013,7 +20767,9 @@
       <c r="F647" t="s">
         <v>538</v>
       </c>
-      <c r="G647"/>
+      <c r="G647" t="n">
+        <v>2</v>
+      </c>
       <c r="H647" t="b">
         <v>0</v>
       </c>
@@ -20156,7 +20912,9 @@
       <c r="F652" t="s">
         <v>542</v>
       </c>
-      <c r="G652"/>
+      <c r="G652" t="n">
+        <v>2</v>
+      </c>
       <c r="H652" t="b">
         <v>0</v>
       </c>
@@ -20183,7 +20941,9 @@
       <c r="F653" t="s">
         <v>543</v>
       </c>
-      <c r="G653"/>
+      <c r="G653" t="n">
+        <v>2</v>
+      </c>
       <c r="H653" t="b">
         <v>0</v>
       </c>
@@ -20239,7 +20999,9 @@
       <c r="F655" t="s">
         <v>545</v>
       </c>
-      <c r="G655"/>
+      <c r="G655" t="n">
+        <v>2</v>
+      </c>
       <c r="H655" t="b">
         <v>0</v>
       </c>
@@ -20266,7 +21028,9 @@
       <c r="F656" t="s">
         <v>546</v>
       </c>
-      <c r="G656"/>
+      <c r="G656" t="n">
+        <v>2</v>
+      </c>
       <c r="H656" t="b">
         <v>0</v>
       </c>
@@ -20293,7 +21057,9 @@
       <c r="F657" t="s">
         <v>36</v>
       </c>
-      <c r="G657"/>
+      <c r="G657" t="n">
+        <v>2</v>
+      </c>
       <c r="H657" t="b">
         <v>0</v>
       </c>
@@ -20407,7 +21173,9 @@
       <c r="F661" t="s">
         <v>550</v>
       </c>
-      <c r="G661"/>
+      <c r="G661" t="n">
+        <v>2</v>
+      </c>
       <c r="H661" t="b">
         <v>0</v>
       </c>

</xml_diff>